<commit_message>
Correction de quelques bouts du rapport
</commit_message>
<xml_diff>
--- a/Simulations/tests/lissage_resultats/donnees.xlsx
+++ b/Simulations/tests/lissage_resultats/donnees.xlsx
@@ -4,12 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="0" windowWidth="25600" windowHeight="14420" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14480" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="TTFF_alea" sheetId="2" r:id="rId1"/>
     <sheet name="PCN_alea" sheetId="5" r:id="rId2"/>
-    <sheet name="Feuil1" sheetId="6" r:id="rId3"/>
+    <sheet name="TTFF" sheetId="7" r:id="rId3"/>
+    <sheet name="PCN" sheetId="8" r:id="rId4"/>
+    <sheet name="LC" sheetId="9" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="lissage" localSheetId="0">TTFF_alea!#REF!</definedName>
@@ -109,7 +111,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="15">
   <si>
     <t>FLOOD</t>
   </si>
@@ -209,8 +211,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="29">
+  <cellStyleXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -244,7 +256,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="29">
+  <cellStyles count="39">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
@@ -259,6 +271,11 @@
     <cellStyle name="Lien hypertexte" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
@@ -273,6 +290,11 @@
     <cellStyle name="Lien hypertexte visité" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -928,11 +950,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2049376040"/>
-        <c:axId val="2049379336"/>
+        <c:axId val="2057144392"/>
+        <c:axId val="2057147528"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2049376040"/>
+        <c:axId val="2057144392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -942,7 +964,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2049379336"/>
+        <c:crossAx val="2057147528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -950,7 +972,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2049379336"/>
+        <c:axId val="2057147528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -961,7 +983,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2049376040"/>
+        <c:crossAx val="2057144392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1631,11 +1653,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2049497768"/>
-        <c:axId val="2049500872"/>
+        <c:axId val="2057198696"/>
+        <c:axId val="2057201800"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2049497768"/>
+        <c:axId val="2057198696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1645,7 +1667,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2049500872"/>
+        <c:crossAx val="2057201800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1653,7 +1675,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2049500872"/>
+        <c:axId val="2057201800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1000.0"/>
@@ -1666,7 +1688,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2049497768"/>
+        <c:crossAx val="2057198696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1713,7 +1735,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Feuil1!$B$1</c:f>
+              <c:f>TTFF!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1727,72 +1749,78 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Feuil1!$A$2:$A$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
+              <c:f>TTFF!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>0.25</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>0.3</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>0.35</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>0.4</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>0.45</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>0.5</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>0.55</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>0.6</c:v>
                 </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.75</c:v>
+                <c:pt idx="9">
+                  <c:v>0.65</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Feuil1!$B$2:$B$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>113.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>113.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>113.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>113.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>113.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>113.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>113.0</c:v>
+              <c:f>TTFF!$B$2:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>447.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>447.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>447.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>447.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>447.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>447.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>447.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>113.0</c:v>
+                  <c:v>447.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>113.0</c:v>
+                  <c:v>447.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>447.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1804,7 +1832,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Feuil1!$C$1</c:f>
+              <c:f>TTFF!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1818,72 +1846,78 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Feuil1!$A$2:$A$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
+              <c:f>TTFF!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>0.25</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>0.3</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>0.35</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>0.4</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>0.45</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>0.5</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>0.55</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>0.6</c:v>
                 </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.75</c:v>
+                <c:pt idx="9">
+                  <c:v>0.65</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Feuil1!$C$2:$C$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>119.4</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>117.667</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>118.333</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>119.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>122.667</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>120.5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>123.5</c:v>
+              <c:f>TTFF!$C$2:$C$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>466.9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>468.379</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>468.038</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>469.909</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>474.667</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>483.182</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>481.885</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>125.0</c:v>
+                  <c:v>486.379</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>133.0</c:v>
+                  <c:v>493.512</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>510.486</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1895,7 +1929,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Feuil1!$D$1</c:f>
+              <c:f>TTFF!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1909,72 +1943,78 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Feuil1!$A$2:$A$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
+              <c:f>TTFF!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>0.25</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>0.3</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>0.35</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>0.4</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>0.45</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>0.5</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>0.55</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>0.6</c:v>
                 </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.75</c:v>
+                <c:pt idx="9">
+                  <c:v>0.65</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Feuil1!$D$2:$D$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>117.4</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>117.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>115.889</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>117.2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>120.667</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>118.5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>124.0</c:v>
+              <c:f>TTFF!$D$2:$D$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>466.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>467.241</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>467.506</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>468.455</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>474.444</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>483.982</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>482.462</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>135.0</c:v>
+                  <c:v>490.448</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>131.0</c:v>
+                  <c:v>499.326</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>512.943</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1986,7 +2026,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Feuil1!$E$1</c:f>
+              <c:f>TTFF!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2000,72 +2040,78 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Feuil1!$A$2:$A$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
+              <c:f>TTFF!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>0.25</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>0.3</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>0.35</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>0.4</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>0.45</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>0.5</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>0.55</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>0.6</c:v>
                 </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.75</c:v>
+                <c:pt idx="9">
+                  <c:v>0.65</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Feuil1!$E$2:$E$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>120.2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>123.222</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>122.556</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>125.8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>128.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>127.5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>127.5</c:v>
+              <c:f>TTFF!$E$2:$E$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>476.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>483.172</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>485.81</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>490.303</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>497.778</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>497.618</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>508.769</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>155.0</c:v>
+                  <c:v>510.241</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>132.0</c:v>
+                  <c:v>518.535</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>541.571</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2077,7 +2123,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Feuil1!$F$1</c:f>
+              <c:f>TTFF!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2091,72 +2137,78 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Feuil1!$A$2:$A$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
+              <c:f>TTFF!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>0.25</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>0.3</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>0.35</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>0.4</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>0.45</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>0.5</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>0.55</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>0.6</c:v>
                 </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.75</c:v>
+                <c:pt idx="9">
+                  <c:v>0.65</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Feuil1!$F$2:$F$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>118.6</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>120.111</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>119.222</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>122.6</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>122.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>121.5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>118.0</c:v>
+              <c:f>TTFF!$F$2:$F$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>473.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>476.448</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>475.43</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>474.364</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>484.167</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>481.364</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>481.692</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>133.0</c:v>
+                  <c:v>483.552</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>120.0</c:v>
+                  <c:v>492.628</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>497.857</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2168,7 +2220,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Feuil1!$G$1</c:f>
+              <c:f>TTFF!$G$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2182,72 +2234,78 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Feuil1!$A$2:$A$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
+              <c:f>TTFF!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>0.25</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>0.3</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>0.35</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>0.4</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>0.45</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>0.5</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>0.55</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>0.6</c:v>
                 </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.75</c:v>
+                <c:pt idx="9">
+                  <c:v>0.65</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Feuil1!$G$2:$G$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>118.6</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>120.111</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>119.222</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>121.8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>121.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>122.5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>120.0</c:v>
+              <c:f>TTFF!$G$2:$G$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>475.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>478.069</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>476.899</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>476.152</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>486.778</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>483.473</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>484.615</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>129.0</c:v>
+                  <c:v>485.069</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>122.0</c:v>
+                  <c:v>495.14</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>499.514</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2264,11 +2322,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2057704904"/>
-        <c:axId val="2057706872"/>
+        <c:axId val="2069127560"/>
+        <c:axId val="2069497528"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2057704904"/>
+        <c:axId val="2069127560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2278,7 +2336,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2057706872"/>
+        <c:crossAx val="2069497528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2286,10 +2344,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2057706872"/>
+        <c:axId val="2069497528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="100.0"/>
+          <c:min val="440.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2298,7 +2356,1161 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2057704904"/>
+        <c:crossAx val="2069127560"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>PCN!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>FLOOD</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>PCN!$A$2:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.55</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>PCN!$B$2:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>447.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>447.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>447.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>447.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>447.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>447.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>447.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>PCN!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>RBOP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>PCN!$A$2:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.55</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>PCN!$C$2:$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>954.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>986.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1062.75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>999.25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>992.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>934.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1001.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>PCN!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>LBOP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>PCN!$A$2:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.55</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>PCN!$D$2:$D$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1214.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>933.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1513.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1533.75</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1020.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1333.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1395.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>PCN!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>BIP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>PCN!$A$2:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.55</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>PCN!$E$2:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>3793.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5553.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5693.75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7283.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5367.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6847.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6269.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>PCN!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>LBIP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>PCN!$A$2:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.55</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>PCN!$F$2:$F$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>945.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1350.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1360.25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1399.75</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1277.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1126.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2081.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>PCN!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>DLBIP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>PCN!$A$2:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.55</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>PCN!$G$2:$G$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>957.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1451.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1594.75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1862.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1141.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1109.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2587.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="2068046936"/>
+        <c:axId val="2068154712"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2068046936"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2068154712"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2068154712"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2068046936"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>LC!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>FLOOD</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>LC!$A$2:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.55</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>LC!$B$2:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>447.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>447.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>447.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>447.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>447.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>447.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>447.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>447.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>LC!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>RBOP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>LC!$A$2:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.55</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>LC!$C$2:$C$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>483.444</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>504.074</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>529.917</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>496.815</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>495.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>491.842</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>550.4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>486.579</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>LC!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>LBOP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>LC!$A$2:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.55</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>LC!$D$2:$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>474.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>482.296</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>492.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>488.333</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>493.875</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>492.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>543.8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>523.947</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>LC!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>BIP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>LC!$A$2:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.55</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>LC!$E$2:$E$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>474.778</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>543.8150000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>507.222</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>518.63</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>541.062</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>547.737</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>573.4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>655.737</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>LC!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>LBIP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>LC!$A$2:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.55</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>LC!$F$2:$F$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>477.889</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>494.296</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>490.667</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>503.704</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>508.938</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>513.789</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>502.533</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>557.947</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>LC!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>DLBIP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>LC!$A$2:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.55</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>LC!$G$2:$G$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>479.778</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>494.481</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>490.972</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>504.444</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>510.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>518.895</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>504.933</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>557.737</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="2069413064"/>
+        <c:axId val="2066623864"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2069413064"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2066623864"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2066623864"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2069413064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2395,15 +3607,85 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>88900</xdr:colOff>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Graphique 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>469900</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Graphique 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3090,7 +4372,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3370,6 +4652,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -3381,10 +4664,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3411,140 +4694,573 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2">
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
       <c r="B2">
-        <v>113</v>
+        <v>447</v>
       </c>
       <c r="C2">
-        <v>119.4</v>
+        <v>466.9</v>
       </c>
       <c r="D2">
-        <v>117.4</v>
+        <v>466.4</v>
       </c>
       <c r="E2">
-        <v>120.2</v>
+        <v>476.5</v>
       </c>
       <c r="F2">
-        <v>118.6</v>
+        <v>473.8</v>
       </c>
       <c r="G2">
-        <v>118.6</v>
+        <v>475.4</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3">
-        <v>0.3</v>
+        <v>0.25</v>
       </c>
       <c r="B3">
-        <v>113</v>
+        <v>447</v>
       </c>
       <c r="C3">
-        <v>117.667</v>
+        <v>468.37900000000002</v>
       </c>
       <c r="D3">
-        <v>117</v>
+        <v>467.24099999999999</v>
       </c>
       <c r="E3">
-        <v>123.22199999999999</v>
+        <v>483.17200000000003</v>
       </c>
       <c r="F3">
-        <v>120.111</v>
+        <v>476.44799999999998</v>
       </c>
       <c r="G3">
-        <v>120.111</v>
+        <v>478.06900000000002</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4">
-        <v>0.35</v>
+        <v>0.3</v>
       </c>
       <c r="B4">
-        <v>113</v>
+        <v>447</v>
       </c>
       <c r="C4">
-        <v>118.333</v>
+        <v>468.03800000000001</v>
       </c>
       <c r="D4">
-        <v>115.889</v>
+        <v>467.50599999999997</v>
       </c>
       <c r="E4">
-        <v>122.556</v>
+        <v>485.81</v>
       </c>
       <c r="F4">
-        <v>119.22199999999999</v>
+        <v>475.43</v>
       </c>
       <c r="G4">
-        <v>119.22199999999999</v>
+        <v>476.899</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5">
-        <v>0.4</v>
+        <v>0.35</v>
       </c>
       <c r="B5">
-        <v>113</v>
+        <v>447</v>
       </c>
       <c r="C5">
-        <v>119</v>
+        <v>469.90899999999999</v>
       </c>
       <c r="D5">
-        <v>117.2</v>
+        <v>468.45499999999998</v>
       </c>
       <c r="E5">
-        <v>125.8</v>
+        <v>490.303</v>
       </c>
       <c r="F5">
-        <v>122.6</v>
+        <v>474.36399999999998</v>
       </c>
       <c r="G5">
-        <v>121.8</v>
+        <v>476.15199999999999</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6">
-        <v>0.45</v>
+        <v>0.4</v>
       </c>
       <c r="B6">
-        <v>113</v>
+        <v>447</v>
       </c>
       <c r="C6">
-        <v>122.667</v>
+        <v>474.66699999999997</v>
       </c>
       <c r="D6">
-        <v>120.667</v>
+        <v>474.44400000000002</v>
       </c>
       <c r="E6">
-        <v>128</v>
+        <v>497.77800000000002</v>
       </c>
       <c r="F6">
-        <v>122</v>
+        <v>484.16699999999997</v>
       </c>
       <c r="G6">
-        <v>121</v>
+        <v>486.77800000000002</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7">
+        <v>0.45</v>
+      </c>
+      <c r="B7">
+        <v>447</v>
+      </c>
+      <c r="C7">
+        <v>483.18200000000002</v>
+      </c>
+      <c r="D7">
+        <v>483.98200000000003</v>
+      </c>
+      <c r="E7">
+        <v>497.61799999999999</v>
+      </c>
+      <c r="F7">
+        <v>481.36399999999998</v>
+      </c>
+      <c r="G7">
+        <v>483.47300000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8">
         <v>0.5</v>
       </c>
+      <c r="B8">
+        <v>447</v>
+      </c>
+      <c r="C8">
+        <v>481.88499999999999</v>
+      </c>
+      <c r="D8">
+        <v>482.46199999999999</v>
+      </c>
+      <c r="E8">
+        <v>508.76900000000001</v>
+      </c>
+      <c r="F8">
+        <v>481.69200000000001</v>
+      </c>
+      <c r="G8">
+        <v>484.61500000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="B9">
+        <v>447</v>
+      </c>
+      <c r="C9">
+        <v>486.37900000000002</v>
+      </c>
+      <c r="D9">
+        <v>490.44799999999998</v>
+      </c>
+      <c r="E9">
+        <v>510.24099999999999</v>
+      </c>
+      <c r="F9">
+        <v>483.55200000000002</v>
+      </c>
+      <c r="G9">
+        <v>485.06900000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10">
+        <v>0.6</v>
+      </c>
+      <c r="B10">
+        <v>447</v>
+      </c>
+      <c r="C10">
+        <v>493.512</v>
+      </c>
+      <c r="D10">
+        <v>499.32600000000002</v>
+      </c>
+      <c r="E10">
+        <v>518.53499999999997</v>
+      </c>
+      <c r="F10">
+        <v>492.62799999999999</v>
+      </c>
+      <c r="G10">
+        <v>495.14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11">
+        <v>0.65</v>
+      </c>
+      <c r="B11">
+        <v>447</v>
+      </c>
+      <c r="C11">
+        <v>510.48599999999999</v>
+      </c>
+      <c r="D11">
+        <v>512.94299999999998</v>
+      </c>
+      <c r="E11">
+        <v>541.57100000000003</v>
+      </c>
+      <c r="F11">
+        <v>497.85700000000003</v>
+      </c>
+      <c r="G11">
+        <v>499.51400000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12">
+        <v>0.7</v>
+      </c>
+      <c r="B12">
+        <v>447</v>
+      </c>
+      <c r="C12">
+        <v>502.161</v>
+      </c>
+      <c r="D12">
+        <v>516.80600000000004</v>
+      </c>
+      <c r="E12">
+        <v>542.09699999999998</v>
+      </c>
+      <c r="F12">
+        <v>491</v>
+      </c>
+      <c r="G12">
+        <v>493.774</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13">
+        <v>0.75</v>
+      </c>
+      <c r="B13">
+        <v>447</v>
+      </c>
+      <c r="C13">
+        <v>501.85700000000003</v>
+      </c>
+      <c r="D13">
+        <v>501</v>
+      </c>
+      <c r="E13">
+        <v>550.14300000000003</v>
+      </c>
+      <c r="F13">
+        <v>499.42899999999997</v>
+      </c>
+      <c r="G13">
+        <v>507.14299999999997</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14">
+        <v>0.8</v>
+      </c>
+      <c r="B14">
+        <v>447</v>
+      </c>
+      <c r="C14">
+        <v>518.11099999999999</v>
+      </c>
+      <c r="D14">
+        <v>537.66700000000003</v>
+      </c>
+      <c r="E14">
+        <v>551.22199999999998</v>
+      </c>
+      <c r="F14">
+        <v>505.22199999999998</v>
+      </c>
+      <c r="G14">
+        <v>507.88900000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15">
+        <v>0.85</v>
+      </c>
+      <c r="B15">
+        <v>447</v>
+      </c>
+      <c r="C15">
+        <v>506.77800000000002</v>
+      </c>
+      <c r="D15">
+        <v>512.33299999999997</v>
+      </c>
+      <c r="E15">
+        <v>532.55600000000004</v>
+      </c>
+      <c r="F15">
+        <v>491.22199999999998</v>
+      </c>
+      <c r="G15">
+        <v>493.88900000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16">
+        <v>0.9</v>
+      </c>
+      <c r="B16">
+        <v>447</v>
+      </c>
+      <c r="C16">
+        <v>523</v>
+      </c>
+      <c r="D16">
+        <v>521</v>
+      </c>
+      <c r="E16">
+        <v>631</v>
+      </c>
+      <c r="F16">
+        <v>471</v>
+      </c>
+      <c r="G16">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17">
+        <v>0.95</v>
+      </c>
+      <c r="B17">
+        <v>447</v>
+      </c>
+      <c r="C17">
+        <v>520</v>
+      </c>
+      <c r="D17">
+        <v>518</v>
+      </c>
+      <c r="E17">
+        <v>572</v>
+      </c>
+      <c r="F17">
+        <v>494</v>
+      </c>
+      <c r="G17">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18">
+        <v>447</v>
+      </c>
+      <c r="C18">
+        <v>511</v>
+      </c>
+      <c r="D18">
+        <v>509</v>
+      </c>
+      <c r="E18">
+        <v>513</v>
+      </c>
+      <c r="F18">
+        <v>515</v>
+      </c>
+      <c r="G18">
+        <v>515</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2">
+        <v>0.2</v>
+      </c>
+      <c r="B2">
+        <v>447</v>
+      </c>
+      <c r="C2">
+        <v>954</v>
+      </c>
+      <c r="D2">
+        <v>1214</v>
+      </c>
+      <c r="E2">
+        <v>3793</v>
+      </c>
+      <c r="F2">
+        <v>945</v>
+      </c>
+      <c r="G2">
+        <v>957</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3">
+        <v>0.25</v>
+      </c>
+      <c r="B3">
+        <v>447</v>
+      </c>
+      <c r="C3">
+        <v>986.5</v>
+      </c>
+      <c r="D3">
+        <v>933</v>
+      </c>
+      <c r="E3">
+        <v>5553</v>
+      </c>
+      <c r="F3">
+        <v>1350.5</v>
+      </c>
+      <c r="G3">
+        <v>1451.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4">
+        <v>0.3</v>
+      </c>
+      <c r="B4">
+        <v>447</v>
+      </c>
+      <c r="C4">
+        <v>1062.75</v>
+      </c>
+      <c r="D4">
+        <v>1513.5</v>
+      </c>
+      <c r="E4">
+        <v>5693.75</v>
+      </c>
+      <c r="F4">
+        <v>1360.25</v>
+      </c>
+      <c r="G4">
+        <v>1594.75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5">
+        <v>0.35</v>
+      </c>
+      <c r="B5">
+        <v>447</v>
+      </c>
+      <c r="C5">
+        <v>999.25</v>
+      </c>
+      <c r="D5">
+        <v>1533.75</v>
+      </c>
+      <c r="E5">
+        <v>7283.5</v>
+      </c>
+      <c r="F5">
+        <v>1399.75</v>
+      </c>
+      <c r="G5">
+        <v>1862</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6">
+        <v>0.4</v>
+      </c>
+      <c r="B6">
+        <v>447</v>
+      </c>
+      <c r="C6">
+        <v>992</v>
+      </c>
+      <c r="D6">
+        <v>1020</v>
+      </c>
+      <c r="E6">
+        <v>5367</v>
+      </c>
+      <c r="F6">
+        <v>1277</v>
+      </c>
+      <c r="G6">
+        <v>1141</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7">
+        <v>0.45</v>
+      </c>
       <c r="B7">
-        <v>113</v>
+        <v>447</v>
       </c>
       <c r="C7">
-        <v>120.5</v>
+        <v>934</v>
       </c>
       <c r="D7">
-        <v>118.5</v>
+        <v>1333</v>
       </c>
       <c r="E7">
-        <v>127.5</v>
+        <v>6847</v>
       </c>
       <c r="F7">
-        <v>121.5</v>
+        <v>1126</v>
       </c>
       <c r="G7">
-        <v>122.5</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -3552,68 +5268,455 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="B8">
-        <v>113</v>
+        <v>447</v>
       </c>
       <c r="C8">
-        <v>123.5</v>
+        <v>1001</v>
       </c>
       <c r="D8">
-        <v>124</v>
+        <v>1395</v>
       </c>
       <c r="E8">
-        <v>127.5</v>
+        <v>6269</v>
       </c>
       <c r="F8">
-        <v>118</v>
+        <v>2081</v>
       </c>
       <c r="G8">
-        <v>120</v>
+        <v>2587</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2">
+        <v>0.2</v>
+      </c>
+      <c r="B2">
+        <v>447</v>
+      </c>
+      <c r="C2">
+        <v>483.44400000000002</v>
+      </c>
+      <c r="D2">
+        <v>474</v>
+      </c>
+      <c r="E2">
+        <v>474.77800000000002</v>
+      </c>
+      <c r="F2">
+        <v>477.88900000000001</v>
+      </c>
+      <c r="G2">
+        <v>479.77800000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3">
+        <v>0.25</v>
+      </c>
+      <c r="B3">
+        <v>447</v>
+      </c>
+      <c r="C3">
+        <v>504.07400000000001</v>
+      </c>
+      <c r="D3">
+        <v>482.29599999999999</v>
+      </c>
+      <c r="E3">
+        <v>543.81500000000005</v>
+      </c>
+      <c r="F3">
+        <v>494.29599999999999</v>
+      </c>
+      <c r="G3">
+        <v>494.48099999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4">
+        <v>0.3</v>
+      </c>
+      <c r="B4">
+        <v>447</v>
+      </c>
+      <c r="C4">
+        <v>529.91700000000003</v>
+      </c>
+      <c r="D4">
+        <v>492.5</v>
+      </c>
+      <c r="E4">
+        <v>507.22199999999998</v>
+      </c>
+      <c r="F4">
+        <v>490.66699999999997</v>
+      </c>
+      <c r="G4">
+        <v>490.97199999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5">
+        <v>0.35</v>
+      </c>
+      <c r="B5">
+        <v>447</v>
+      </c>
+      <c r="C5">
+        <v>496.815</v>
+      </c>
+      <c r="D5">
+        <v>488.33300000000003</v>
+      </c>
+      <c r="E5">
+        <v>518.63</v>
+      </c>
+      <c r="F5">
+        <v>503.70400000000001</v>
+      </c>
+      <c r="G5">
+        <v>504.44400000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6">
+        <v>0.4</v>
+      </c>
+      <c r="B6">
+        <v>447</v>
+      </c>
+      <c r="C6">
+        <v>495</v>
+      </c>
+      <c r="D6">
+        <v>493.875</v>
+      </c>
+      <c r="E6">
+        <v>541.06200000000001</v>
+      </c>
+      <c r="F6">
+        <v>508.93799999999999</v>
+      </c>
+      <c r="G6">
+        <v>510.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7">
+        <v>0.45</v>
+      </c>
+      <c r="B7">
+        <v>447</v>
+      </c>
+      <c r="C7">
+        <v>491.84199999999998</v>
+      </c>
+      <c r="D7">
+        <v>492</v>
+      </c>
+      <c r="E7">
+        <v>547.73699999999997</v>
+      </c>
+      <c r="F7">
+        <v>513.78899999999999</v>
+      </c>
+      <c r="G7">
+        <v>518.89499999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8">
+        <v>0.5</v>
+      </c>
+      <c r="B8">
+        <v>447</v>
+      </c>
+      <c r="C8">
+        <v>550.4</v>
+      </c>
+      <c r="D8">
+        <v>543.79999999999995</v>
+      </c>
+      <c r="E8">
+        <v>573.4</v>
+      </c>
+      <c r="F8">
+        <v>502.53300000000002</v>
+      </c>
+      <c r="G8">
+        <v>504.93299999999999</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9">
-        <v>0.6</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="B9">
-        <v>113</v>
+        <v>447</v>
       </c>
       <c r="C9">
-        <v>125</v>
+        <v>486.57900000000001</v>
       </c>
       <c r="D9">
-        <v>135</v>
+        <v>523.947</v>
       </c>
       <c r="E9">
-        <v>155</v>
+        <v>655.73699999999997</v>
       </c>
       <c r="F9">
-        <v>133</v>
+        <v>557.947</v>
       </c>
       <c r="G9">
-        <v>129</v>
+        <v>557.73699999999997</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10">
+        <v>0.6</v>
+      </c>
+      <c r="B10">
+        <v>447</v>
+      </c>
+      <c r="C10">
+        <v>535</v>
+      </c>
+      <c r="D10">
+        <v>552.93299999999999</v>
+      </c>
+      <c r="E10">
+        <v>532.26700000000005</v>
+      </c>
+      <c r="F10">
+        <v>532.66700000000003</v>
+      </c>
+      <c r="G10">
+        <v>533.46699999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11">
+        <v>0.65</v>
+      </c>
+      <c r="B11">
+        <v>447</v>
+      </c>
+      <c r="C11">
+        <v>735.72</v>
+      </c>
+      <c r="D11">
+        <v>556.04</v>
+      </c>
+      <c r="E11">
+        <v>597.48</v>
+      </c>
+      <c r="F11">
+        <v>534.76</v>
+      </c>
+      <c r="G11">
+        <v>530.20000000000005</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12">
+        <v>0.7</v>
+      </c>
+      <c r="B12">
+        <v>447</v>
+      </c>
+      <c r="C12">
+        <v>562.54499999999996</v>
+      </c>
+      <c r="D12">
+        <v>552.36400000000003</v>
+      </c>
+      <c r="E12">
+        <v>798.54499999999996</v>
+      </c>
+      <c r="F12">
+        <v>601.36400000000003</v>
+      </c>
+      <c r="G12">
+        <v>589.36400000000003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13">
         <v>0.75</v>
       </c>
-      <c r="B10">
-        <v>113</v>
-      </c>
-      <c r="C10">
-        <v>133</v>
-      </c>
-      <c r="D10">
-        <v>131</v>
-      </c>
-      <c r="E10">
-        <v>132</v>
-      </c>
-      <c r="F10">
-        <v>120</v>
-      </c>
-      <c r="G10">
-        <v>122</v>
+      <c r="B13">
+        <v>447</v>
+      </c>
+      <c r="C13">
+        <v>590.63599999999997</v>
+      </c>
+      <c r="D13">
+        <v>510.27300000000002</v>
+      </c>
+      <c r="E13">
+        <v>1093</v>
+      </c>
+      <c r="F13">
+        <v>586.81799999999998</v>
+      </c>
+      <c r="G13">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14">
+        <v>0.8</v>
+      </c>
+      <c r="B14">
+        <v>447</v>
+      </c>
+      <c r="C14">
+        <v>475.66699999999997</v>
+      </c>
+      <c r="D14">
+        <v>826.33299999999997</v>
+      </c>
+      <c r="E14">
+        <v>3943.67</v>
+      </c>
+      <c r="F14">
+        <v>634.33299999999997</v>
+      </c>
+      <c r="G14">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15">
+        <v>0.85</v>
+      </c>
+      <c r="B15">
+        <v>447</v>
+      </c>
+      <c r="C15">
+        <v>509</v>
+      </c>
+      <c r="D15">
+        <v>746.25</v>
+      </c>
+      <c r="E15">
+        <v>2100</v>
+      </c>
+      <c r="F15">
+        <v>545.75</v>
+      </c>
+      <c r="G15">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16">
+        <v>0.9</v>
+      </c>
+      <c r="B16">
+        <v>447</v>
+      </c>
+      <c r="C16">
+        <v>637</v>
+      </c>
+      <c r="D16">
+        <v>687</v>
+      </c>
+      <c r="E16">
+        <v>9719</v>
+      </c>
+      <c r="F16">
+        <v>593</v>
+      </c>
+      <c r="G16">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17">
+        <v>0.95</v>
+      </c>
+      <c r="B17">
+        <v>447</v>
+      </c>
+      <c r="C17">
+        <v>449</v>
+      </c>
+      <c r="D17">
+        <v>525</v>
+      </c>
+      <c r="E17">
+        <v>529</v>
+      </c>
+      <c r="F17">
+        <v>535</v>
+      </c>
+      <c r="G17">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18">
+        <v>447</v>
+      </c>
+      <c r="C18">
+        <v>453</v>
+      </c>
+      <c r="D18">
+        <v>509</v>
+      </c>
+      <c r="E18">
+        <v>513</v>
+      </c>
+      <c r="F18">
+        <v>515</v>
+      </c>
+      <c r="G18">
+        <v>515</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Exemples ShowGraphe pour Rabah
</commit_message>
<xml_diff>
--- a/Simulations/tests/lissage_resultats/donnees.xlsx
+++ b/Simulations/tests/lissage_resultats/donnees.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14480" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14480" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="TTFF_alea" sheetId="7" r:id="rId1"/>
@@ -2392,37 +2392,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>571.746</c:v>
+                  <c:v>571.467</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>573.232</c:v>
+                  <c:v>573.756</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>574.7</c:v>
+                  <c:v>574.288</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>580.256</c:v>
+                  <c:v>582.456</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>584.696</c:v>
+                  <c:v>583.625</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>593.452</c:v>
+                  <c:v>591.271</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>591.708</c:v>
+                  <c:v>593.633</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>595.92</c:v>
+                  <c:v>594.667</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>591.667</c:v>
+                  <c:v>593.462</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>587.8</c:v>
+                  <c:v>586.8819999999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>600.2</c:v>
+                  <c:v>602.158</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2495,37 +2495,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>569.678</c:v>
+                  <c:v>569.4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>572.393</c:v>
+                  <c:v>572.849</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>573.68</c:v>
+                  <c:v>573.119</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>580.302</c:v>
+                  <c:v>582.592</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>582.772</c:v>
+                  <c:v>581.688</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>596.429</c:v>
+                  <c:v>593.625</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>594.631</c:v>
+                  <c:v>596.468</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>601.92</c:v>
+                  <c:v>600.074</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>591.25</c:v>
+                  <c:v>596.692</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>600.2</c:v>
+                  <c:v>597.588</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>598.867</c:v>
+                  <c:v>606.579</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2598,37 +2598,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>574.051</c:v>
+                  <c:v>573.7329999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>575.429</c:v>
+                  <c:v>575.487</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>579.3</c:v>
+                  <c:v>578.525</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>584.047</c:v>
+                  <c:v>586.126</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>588.696</c:v>
+                  <c:v>588.396</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>597.024</c:v>
+                  <c:v>595.854</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>589.615</c:v>
+                  <c:v>592.975</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>610.8</c:v>
+                  <c:v>609.074</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>599.917</c:v>
+                  <c:v>600.538</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>618.6</c:v>
+                  <c:v>621.941</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>619.667</c:v>
+                  <c:v>614.789</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2701,37 +2701,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>565.576</c:v>
+                  <c:v>565.367</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>566.946</c:v>
+                  <c:v>567.084</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>568.0599999999999</c:v>
+                  <c:v>567.576</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>571.419</c:v>
+                  <c:v>571.2329999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>571.684</c:v>
+                  <c:v>572.021</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>575.048</c:v>
+                  <c:v>574.667</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>575.246</c:v>
+                  <c:v>575.886</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>576.08</c:v>
+                  <c:v>576.222</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>576.75</c:v>
+                  <c:v>576.769</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>576.6</c:v>
+                  <c:v>576.412</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>583.933</c:v>
+                  <c:v>580.684</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2804,37 +2804,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>566.695</c:v>
+                  <c:v>566.467</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>568.107</c:v>
+                  <c:v>568.328</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>569.16</c:v>
+                  <c:v>568.542</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>572.163</c:v>
+                  <c:v>571.854</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>572.468</c:v>
+                  <c:v>573.104</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>576.619</c:v>
+                  <c:v>576.25</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>577.431</c:v>
+                  <c:v>578.848</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>577.88</c:v>
+                  <c:v>577.889</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>580.083</c:v>
+                  <c:v>579.923</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>576.333</c:v>
+                  <c:v>576.059</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>589.667</c:v>
+                  <c:v>586.263</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2946,46 +2946,52 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>PCN_alea_real!$A$3:$A$11</c:f>
+              <c:f>PCN_alea_real!$A$2:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>0.25</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>0.3</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>0.35</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>0.4</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>0.45</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>0.5</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>0.55</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>0.6</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>PCN_alea_real!$B$3:$B$11</c:f>
+              <c:f>PCN_alea_real!$B$2:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>555.0</c:v>
                 </c:pt>
@@ -3011,6 +3017,12 @@
                   <c:v>555.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>555.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>555.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>555.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -3037,72 +3049,84 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>PCN_alea_real!$A$3:$A$11</c:f>
+              <c:f>PCN_alea_real!$A$2:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>0.25</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>0.3</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>0.35</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>0.4</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>0.45</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>0.5</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>0.55</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>0.6</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>PCN_alea_real!$C$3:$C$11</c:f>
+              <c:f>PCN_alea_real!$C$2:$C$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>920.5</c:v>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>871.2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1029.67</c:v>
+                  <c:v>908.111</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>919.667</c:v>
+                  <c:v>995.667</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>893.0</c:v>
+                  <c:v>904.429</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>931.0</c:v>
+                  <c:v>918.714</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>927.889</c:v>
+                  <c:v>926.429</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>974.818</c:v>
+                  <c:v>920.273</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>963.167</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>915.25</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>935.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>923.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3128,72 +3152,84 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>PCN_alea_real!$A$3:$A$11</c:f>
+              <c:f>PCN_alea_real!$A$2:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>0.25</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>0.3</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>0.35</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>0.4</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>0.45</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>0.5</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>0.55</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>0.6</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>PCN_alea_real!$D$3:$D$11</c:f>
+              <c:f>PCN_alea_real!$D$2:$D$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>1039.62</c:v>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>961.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>955.667</c:v>
+                  <c:v>1027.22</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1249.67</c:v>
+                  <c:v>995.222</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>925.0</c:v>
+                  <c:v>1111.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1021.36</c:v>
+                  <c:v>1001.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>966.333</c:v>
+                  <c:v>1013.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1019.36</c:v>
+                  <c:v>988.818</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>1009.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>1017.75</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>1015.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1051.4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3219,72 +3255,84 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>PCN_alea_real!$A$3:$A$11</c:f>
+              <c:f>PCN_alea_real!$A$2:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>0.25</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>0.3</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>0.35</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>0.4</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>0.45</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>0.5</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>0.55</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>0.6</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>PCN_alea_real!$E$3:$E$11</c:f>
+              <c:f>PCN_alea_real!$E$2:$E$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>3056.25</c:v>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>3365.8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2441.0</c:v>
+                  <c:v>3079.11</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3101.67</c:v>
+                  <c:v>2843.67</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3085.0</c:v>
+                  <c:v>3271.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3711.73</c:v>
+                  <c:v>3351.57</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3263.44</c:v>
+                  <c:v>3632.86</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3585.18</c:v>
+                  <c:v>3397.91</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>3579.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>3676.5</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>3291.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4528.6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3310,72 +3358,84 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>PCN_alea_real!$A$3:$A$11</c:f>
+              <c:f>PCN_alea_real!$A$2:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>0.25</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>0.3</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>0.35</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>0.4</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>0.45</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>0.5</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>0.55</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>0.6</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>PCN_alea_real!$F$3:$F$11</c:f>
+              <c:f>PCN_alea_real!$F$2:$F$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>1450.75</c:v>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1426.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1067.0</c:v>
+                  <c:v>1427.56</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1107.0</c:v>
+                  <c:v>1260.78</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1082.33</c:v>
+                  <c:v>1394.14</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1322.09</c:v>
+                  <c:v>1232.43</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1226.78</c:v>
+                  <c:v>1333.43</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1384.82</c:v>
+                  <c:v>1250.45</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>1356.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>1401.5</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>1359.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1755.4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3401,72 +3461,84 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>PCN_alea_real!$A$3:$A$11</c:f>
+              <c:f>PCN_alea_real!$A$2:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>0.25</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>0.3</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>0.35</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>0.4</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>0.45</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>0.5</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>0.55</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>0.6</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>PCN_alea_real!$G$3:$G$11</c:f>
+              <c:f>PCN_alea_real!$G$2:$G$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>1667.25</c:v>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1601.4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1326.33</c:v>
+                  <c:v>1651.11</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1359.0</c:v>
+                  <c:v>1458.11</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1046.33</c:v>
+                  <c:v>1649.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1401.0</c:v>
+                  <c:v>1331.29</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1394.33</c:v>
+                  <c:v>1423.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1521.36</c:v>
+                  <c:v>1425.36</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>1474.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>1484.5</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>1682.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2076.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3577,44 +3649,41 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>LC_alea_real!$A$2:$A$13</c:f>
+              <c:f>LC_alea_real!$A$3:$A$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>0.15</c:v>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.2</c:v>
+                  <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.25</c:v>
+                  <c:v>0.3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.3</c:v>
+                  <c:v>0.35</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.35</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.4</c:v>
+                  <c:v>0.45</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.45</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.5</c:v>
+                  <c:v>0.55</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.55</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.6</c:v>
+                  <c:v>0.65</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.65</c:v>
-                </c:pt>
-                <c:pt idx="11">
                   <c:v>0.7</c:v>
                 </c:pt>
               </c:numCache>
@@ -3622,10 +3691,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>LC_alea_real!$B$2:$B$13</c:f>
+              <c:f>LC_alea_real!$B$3:$B$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>555.0</c:v>
                 </c:pt>
@@ -3657,9 +3726,6 @@
                   <c:v>555.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>555.0</c:v>
-                </c:pt>
-                <c:pt idx="11">
                   <c:v>555.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -3686,44 +3752,41 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>LC_alea_real!$A$2:$A$13</c:f>
+              <c:f>LC_alea_real!$A$3:$A$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>0.15</c:v>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.2</c:v>
+                  <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.25</c:v>
+                  <c:v>0.3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.3</c:v>
+                  <c:v>0.35</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.35</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.4</c:v>
+                  <c:v>0.45</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.45</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.5</c:v>
+                  <c:v>0.55</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.55</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.6</c:v>
+                  <c:v>0.65</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.65</c:v>
-                </c:pt>
-                <c:pt idx="11">
                   <c:v>0.7</c:v>
                 </c:pt>
               </c:numCache>
@@ -3731,45 +3794,42 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>LC_alea_real!$C$2:$C$13</c:f>
+              <c:f>LC_alea_real!$C$3:$C$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>582.333</c:v>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>603.966</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>603.386</c:v>
+                  <c:v>633.768</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>635.819</c:v>
+                  <c:v>620.709</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>620.83</c:v>
+                  <c:v>599.215</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>600.846</c:v>
+                  <c:v>606.644</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>611.0</c:v>
+                  <c:v>626.506</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>627.722</c:v>
+                  <c:v>609.606</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>612.571</c:v>
+                  <c:v>595.75</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>597.273</c:v>
+                  <c:v>596.1</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>596.1</c:v>
+                  <c:v>590.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>591.444</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>608.0</c:v>
+                  <c:v>613.875</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3795,44 +3855,41 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>LC_alea_real!$A$2:$A$13</c:f>
+              <c:f>LC_alea_real!$A$3:$A$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>0.15</c:v>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.2</c:v>
+                  <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.25</c:v>
+                  <c:v>0.3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.3</c:v>
+                  <c:v>0.35</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.35</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.4</c:v>
+                  <c:v>0.45</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.45</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.5</c:v>
+                  <c:v>0.55</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.55</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.6</c:v>
+                  <c:v>0.65</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.65</c:v>
-                </c:pt>
-                <c:pt idx="11">
                   <c:v>0.7</c:v>
                 </c:pt>
               </c:numCache>
@@ -3840,45 +3897,42 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>LC_alea_real!$D$2:$D$13</c:f>
+              <c:f>LC_alea_real!$D$3:$D$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>577.0</c:v>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>580.414</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>580.895</c:v>
+                  <c:v>585.589</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>584.657</c:v>
+                  <c:v>596.9640000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>596.319</c:v>
+                  <c:v>600.978</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>594.718</c:v>
+                  <c:v>603.311</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>604.432</c:v>
+                  <c:v>621.519</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>624.0</c:v>
+                  <c:v>623.212</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>626.179</c:v>
+                  <c:v>631.25</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>632.636</c:v>
+                  <c:v>622.1</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>622.1</c:v>
+                  <c:v>627.6</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>633.667</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>650.833</c:v>
+                  <c:v>656.125</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3904,44 +3958,41 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>LC_alea_real!$A$2:$A$13</c:f>
+              <c:f>LC_alea_real!$A$3:$A$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>0.15</c:v>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.2</c:v>
+                  <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.25</c:v>
+                  <c:v>0.3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.3</c:v>
+                  <c:v>0.35</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.35</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.4</c:v>
+                  <c:v>0.45</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.45</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.5</c:v>
+                  <c:v>0.55</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.55</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.6</c:v>
+                  <c:v>0.65</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.65</c:v>
-                </c:pt>
-                <c:pt idx="11">
                   <c:v>0.7</c:v>
                 </c:pt>
               </c:numCache>
@@ -3949,45 +4000,42 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>LC_alea_real!$E$2:$E$13</c:f>
+              <c:f>LC_alea_real!$E$3:$E$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>579.0</c:v>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>577.069</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>577.456</c:v>
+                  <c:v>582.804</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>582.886</c:v>
+                  <c:v>594.018</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>593.957</c:v>
+                  <c:v>592.527</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>591.487</c:v>
+                  <c:v>657.8440000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>656.7569999999999</c:v>
+                  <c:v>635.84</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>639.361</c:v>
+                  <c:v>739.576</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>734.071</c:v>
+                  <c:v>643.75</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>648.864</c:v>
+                  <c:v>674.6</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>674.6</c:v>
+                  <c:v>649.2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>657.444</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>732.5</c:v>
+                  <c:v>758.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4013,44 +4061,41 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>LC_alea_real!$A$2:$A$13</c:f>
+              <c:f>LC_alea_real!$A$3:$A$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>0.15</c:v>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.2</c:v>
+                  <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.25</c:v>
+                  <c:v>0.3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.3</c:v>
+                  <c:v>0.35</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.35</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.4</c:v>
+                  <c:v>0.45</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.45</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.5</c:v>
+                  <c:v>0.55</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.55</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.6</c:v>
+                  <c:v>0.65</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.65</c:v>
-                </c:pt>
-                <c:pt idx="11">
                   <c:v>0.7</c:v>
                 </c:pt>
               </c:numCache>
@@ -4058,45 +4103,42 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>LC_alea_real!$F$2:$F$13</c:f>
+              <c:f>LC_alea_real!$F$3:$F$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>577.0</c:v>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>573.379</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>573.737</c:v>
+                  <c:v>577.214</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>576.943</c:v>
+                  <c:v>586.182</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>585.723</c:v>
+                  <c:v>587.28</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>586.308</c:v>
+                  <c:v>591.9109999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>591.973</c:v>
+                  <c:v>601.272</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>602.444</c:v>
+                  <c:v>621.303</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>613.143</c:v>
+                  <c:v>620.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>623.682</c:v>
+                  <c:v>613.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>613.0</c:v>
+                  <c:v>657.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>666.333</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>632.167</c:v>
+                  <c:v>650.125</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4122,44 +4164,41 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>LC_alea_real!$A$2:$A$13</c:f>
+              <c:f>LC_alea_real!$A$3:$A$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>0.15</c:v>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.2</c:v>
+                  <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.25</c:v>
+                  <c:v>0.3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.3</c:v>
+                  <c:v>0.35</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.35</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.4</c:v>
+                  <c:v>0.45</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.45</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.5</c:v>
+                  <c:v>0.55</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.55</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.6</c:v>
+                  <c:v>0.65</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.65</c:v>
-                </c:pt>
-                <c:pt idx="11">
                   <c:v>0.7</c:v>
                 </c:pt>
               </c:numCache>
@@ -4167,45 +4206,42 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>LC_alea_real!$G$2:$G$13</c:f>
+              <c:f>LC_alea_real!$G$3:$G$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>577.0</c:v>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>573.897</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>574.263</c:v>
+                  <c:v>578.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>577.781</c:v>
+                  <c:v>585.855</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>585.383</c:v>
+                  <c:v>586.742</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>585.718</c:v>
+                  <c:v>593.022</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>593.081</c:v>
+                  <c:v>602.852</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>604.111</c:v>
+                  <c:v>615.485</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>608.893</c:v>
+                  <c:v>619.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>622.545</c:v>
+                  <c:v>612.8</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>612.8</c:v>
+                  <c:v>641.6</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>649.222</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>632.167</c:v>
+                  <c:v>655.625</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5290,7 +5326,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
@@ -5973,7 +6009,7 @@
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6029,19 +6065,19 @@
         <v>555</v>
       </c>
       <c r="C3">
-        <v>571.74599999999998</v>
+        <v>571.46699999999998</v>
       </c>
       <c r="D3">
-        <v>569.678</v>
+        <v>569.4</v>
       </c>
       <c r="E3">
-        <v>574.05100000000004</v>
+        <v>573.73299999999995</v>
       </c>
       <c r="F3">
-        <v>565.57600000000002</v>
+        <v>565.36699999999996</v>
       </c>
       <c r="G3">
-        <v>566.69500000000005</v>
+        <v>566.46699999999998</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -6052,19 +6088,19 @@
         <v>555</v>
       </c>
       <c r="C4">
-        <v>573.23199999999997</v>
+        <v>573.75599999999997</v>
       </c>
       <c r="D4">
-        <v>572.39300000000003</v>
+        <v>572.84900000000005</v>
       </c>
       <c r="E4">
-        <v>575.42899999999997</v>
+        <v>575.48699999999997</v>
       </c>
       <c r="F4">
-        <v>566.94600000000003</v>
+        <v>567.08399999999995</v>
       </c>
       <c r="G4">
-        <v>568.10699999999997</v>
+        <v>568.32799999999997</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -6075,19 +6111,19 @@
         <v>555</v>
       </c>
       <c r="C5">
-        <v>574.70000000000005</v>
+        <v>574.28800000000001</v>
       </c>
       <c r="D5">
-        <v>573.67999999999995</v>
+        <v>573.11900000000003</v>
       </c>
       <c r="E5">
-        <v>579.29999999999995</v>
+        <v>578.52499999999998</v>
       </c>
       <c r="F5">
-        <v>568.05999999999995</v>
+        <v>567.57600000000002</v>
       </c>
       <c r="G5">
-        <v>569.16</v>
+        <v>568.54200000000003</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -6098,19 +6134,19 @@
         <v>555</v>
       </c>
       <c r="C6">
-        <v>580.25599999999997</v>
+        <v>582.45600000000002</v>
       </c>
       <c r="D6">
-        <v>580.30200000000002</v>
+        <v>582.59199999999998</v>
       </c>
       <c r="E6">
-        <v>584.04700000000003</v>
+        <v>586.12599999999998</v>
       </c>
       <c r="F6">
-        <v>571.41899999999998</v>
+        <v>571.23299999999995</v>
       </c>
       <c r="G6">
-        <v>572.16300000000001</v>
+        <v>571.85400000000004</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -6121,19 +6157,19 @@
         <v>555</v>
       </c>
       <c r="C7">
-        <v>584.69600000000003</v>
+        <v>583.625</v>
       </c>
       <c r="D7">
-        <v>582.77200000000005</v>
+        <v>581.68799999999999</v>
       </c>
       <c r="E7">
-        <v>588.69600000000003</v>
+        <v>588.39599999999996</v>
       </c>
       <c r="F7">
-        <v>571.68399999999997</v>
+        <v>572.02099999999996</v>
       </c>
       <c r="G7">
-        <v>572.46799999999996</v>
+        <v>573.10400000000004</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -6144,19 +6180,19 @@
         <v>555</v>
       </c>
       <c r="C8">
-        <v>593.452</v>
+        <v>591.27099999999996</v>
       </c>
       <c r="D8">
-        <v>596.42899999999997</v>
+        <v>593.625</v>
       </c>
       <c r="E8">
-        <v>597.024</v>
+        <v>595.85400000000004</v>
       </c>
       <c r="F8">
-        <v>575.048</v>
+        <v>574.66700000000003</v>
       </c>
       <c r="G8">
-        <v>576.61900000000003</v>
+        <v>576.25</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -6167,19 +6203,19 @@
         <v>555</v>
       </c>
       <c r="C9">
-        <v>591.70799999999997</v>
+        <v>593.63300000000004</v>
       </c>
       <c r="D9">
-        <v>594.63099999999997</v>
+        <v>596.46799999999996</v>
       </c>
       <c r="E9">
-        <v>589.61500000000001</v>
+        <v>592.97500000000002</v>
       </c>
       <c r="F9">
-        <v>575.24599999999998</v>
+        <v>575.88599999999997</v>
       </c>
       <c r="G9">
-        <v>577.43100000000004</v>
+        <v>578.84799999999996</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -6190,19 +6226,19 @@
         <v>555</v>
       </c>
       <c r="C10">
-        <v>595.91999999999996</v>
+        <v>594.66700000000003</v>
       </c>
       <c r="D10">
-        <v>601.91999999999996</v>
+        <v>600.07399999999996</v>
       </c>
       <c r="E10">
-        <v>610.79999999999995</v>
+        <v>609.07399999999996</v>
       </c>
       <c r="F10">
-        <v>576.08000000000004</v>
+        <v>576.22199999999998</v>
       </c>
       <c r="G10">
-        <v>577.88</v>
+        <v>577.88900000000001</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -6213,19 +6249,19 @@
         <v>555</v>
       </c>
       <c r="C11">
-        <v>591.66700000000003</v>
+        <v>593.46199999999999</v>
       </c>
       <c r="D11">
-        <v>591.25</v>
+        <v>596.69200000000001</v>
       </c>
       <c r="E11">
-        <v>599.91700000000003</v>
+        <v>600.53800000000001</v>
       </c>
       <c r="F11">
-        <v>576.75</v>
+        <v>576.76900000000001</v>
       </c>
       <c r="G11">
-        <v>580.08299999999997</v>
+        <v>579.923</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -6236,19 +6272,19 @@
         <v>555</v>
       </c>
       <c r="C12">
-        <v>587.79999999999995</v>
+        <v>586.88199999999995</v>
       </c>
       <c r="D12">
-        <v>600.20000000000005</v>
+        <v>597.58799999999997</v>
       </c>
       <c r="E12">
-        <v>618.6</v>
+        <v>621.94100000000003</v>
       </c>
       <c r="F12">
-        <v>576.6</v>
+        <v>576.41200000000003</v>
       </c>
       <c r="G12">
-        <v>576.33299999999997</v>
+        <v>576.05899999999997</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -6259,19 +6295,19 @@
         <v>555</v>
       </c>
       <c r="C13">
-        <v>600.20000000000005</v>
+        <v>602.15800000000002</v>
       </c>
       <c r="D13">
-        <v>598.86699999999996</v>
+        <v>606.57899999999995</v>
       </c>
       <c r="E13">
-        <v>619.66700000000003</v>
+        <v>614.78899999999999</v>
       </c>
       <c r="F13">
-        <v>583.93299999999999</v>
+        <v>580.68399999999997</v>
       </c>
       <c r="G13">
-        <v>589.66700000000003</v>
+        <v>586.26300000000003</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -6282,19 +6318,19 @@
         <v>555</v>
       </c>
       <c r="C14">
-        <v>630.20000000000005</v>
+        <v>648.33299999999997</v>
       </c>
       <c r="D14">
-        <v>642.6</v>
+        <v>669.33299999999997</v>
       </c>
       <c r="E14">
-        <v>598.6</v>
+        <v>621.66700000000003</v>
       </c>
       <c r="F14">
-        <v>612.20000000000005</v>
+        <v>616</v>
       </c>
       <c r="G14">
-        <v>603.79999999999995</v>
+        <v>608</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -6305,19 +6341,19 @@
         <v>555</v>
       </c>
       <c r="C15">
-        <v>637</v>
+        <v>649</v>
       </c>
       <c r="D15">
-        <v>635</v>
+        <v>647</v>
       </c>
       <c r="E15">
-        <v>635</v>
+        <v>639</v>
       </c>
       <c r="F15">
-        <v>589</v>
+        <v>614</v>
       </c>
       <c r="G15">
-        <v>571</v>
+        <v>604</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -6405,7 +6441,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6461,19 +6497,19 @@
         <v>555</v>
       </c>
       <c r="C3">
-        <v>920.5</v>
+        <v>908.11099999999999</v>
       </c>
       <c r="D3">
-        <v>1039.6199999999999</v>
+        <v>1027.22</v>
       </c>
       <c r="E3">
-        <v>3056.25</v>
+        <v>3079.11</v>
       </c>
       <c r="F3">
-        <v>1450.75</v>
+        <v>1427.56</v>
       </c>
       <c r="G3">
-        <v>1667.25</v>
+        <v>1651.11</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -6484,19 +6520,19 @@
         <v>555</v>
       </c>
       <c r="C4">
-        <v>1029.67</v>
+        <v>995.66700000000003</v>
       </c>
       <c r="D4">
-        <v>955.66700000000003</v>
+        <v>995.22199999999998</v>
       </c>
       <c r="E4">
-        <v>2441</v>
+        <v>2843.67</v>
       </c>
       <c r="F4">
-        <v>1067</v>
+        <v>1260.78</v>
       </c>
       <c r="G4">
-        <v>1326.33</v>
+        <v>1458.11</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -6507,19 +6543,19 @@
         <v>555</v>
       </c>
       <c r="C5">
-        <v>919.66700000000003</v>
+        <v>904.42899999999997</v>
       </c>
       <c r="D5">
-        <v>1249.67</v>
+        <v>1111</v>
       </c>
       <c r="E5">
-        <v>3101.67</v>
+        <v>3271</v>
       </c>
       <c r="F5">
-        <v>1107</v>
+        <v>1394.14</v>
       </c>
       <c r="G5">
-        <v>1359</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -6530,19 +6566,19 @@
         <v>555</v>
       </c>
       <c r="C6">
-        <v>893</v>
+        <v>918.71400000000006</v>
       </c>
       <c r="D6">
-        <v>925</v>
+        <v>1001</v>
       </c>
       <c r="E6">
-        <v>3085</v>
+        <v>3351.57</v>
       </c>
       <c r="F6">
-        <v>1082.33</v>
+        <v>1232.43</v>
       </c>
       <c r="G6">
-        <v>1046.33</v>
+        <v>1331.29</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -6553,19 +6589,19 @@
         <v>555</v>
       </c>
       <c r="C7">
-        <v>931</v>
+        <v>926.42899999999997</v>
       </c>
       <c r="D7">
-        <v>1021.36</v>
+        <v>1013</v>
       </c>
       <c r="E7">
-        <v>3711.73</v>
+        <v>3632.86</v>
       </c>
       <c r="F7">
-        <v>1322.09</v>
+        <v>1333.43</v>
       </c>
       <c r="G7">
-        <v>1401</v>
+        <v>1423</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -6576,19 +6612,19 @@
         <v>555</v>
       </c>
       <c r="C8">
-        <v>927.88900000000001</v>
+        <v>920.27300000000002</v>
       </c>
       <c r="D8">
-        <v>966.33299999999997</v>
+        <v>988.81799999999998</v>
       </c>
       <c r="E8">
-        <v>3263.44</v>
+        <v>3397.91</v>
       </c>
       <c r="F8">
-        <v>1226.78</v>
+        <v>1250.45</v>
       </c>
       <c r="G8">
-        <v>1394.33</v>
+        <v>1425.36</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -6599,19 +6635,19 @@
         <v>555</v>
       </c>
       <c r="C9">
-        <v>974.81799999999998</v>
+        <v>963.16700000000003</v>
       </c>
       <c r="D9">
-        <v>1019.36</v>
+        <v>1009.5</v>
       </c>
       <c r="E9">
-        <v>3585.18</v>
+        <v>3579.5</v>
       </c>
       <c r="F9">
-        <v>1384.82</v>
+        <v>1356</v>
       </c>
       <c r="G9">
-        <v>1521.36</v>
+        <v>1474</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -6668,19 +6704,19 @@
         <v>555</v>
       </c>
       <c r="C12">
-        <v>927.66700000000003</v>
+        <v>923</v>
       </c>
       <c r="D12">
-        <v>1099.67</v>
+        <v>1051.4000000000001</v>
       </c>
       <c r="E12">
-        <v>4771.67</v>
+        <v>4528.6000000000004</v>
       </c>
       <c r="F12">
-        <v>1873.67</v>
+        <v>1755.4</v>
       </c>
       <c r="G12">
-        <v>2295.67</v>
+        <v>2076.1999999999998</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -6768,8 +6804,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6825,19 +6861,19 @@
         <v>555</v>
       </c>
       <c r="C3">
-        <v>603.38599999999997</v>
+        <v>603.96600000000001</v>
       </c>
       <c r="D3">
-        <v>580.89499999999998</v>
+        <v>580.41399999999999</v>
       </c>
       <c r="E3">
-        <v>577.45600000000002</v>
+        <v>577.06899999999996</v>
       </c>
       <c r="F3">
-        <v>573.73699999999997</v>
+        <v>573.37900000000002</v>
       </c>
       <c r="G3">
-        <v>574.26300000000003</v>
+        <v>573.89700000000005</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -6848,19 +6884,19 @@
         <v>555</v>
       </c>
       <c r="C4">
-        <v>635.81899999999996</v>
+        <v>633.76800000000003</v>
       </c>
       <c r="D4">
-        <v>584.65700000000004</v>
+        <v>585.58900000000006</v>
       </c>
       <c r="E4">
-        <v>582.88599999999997</v>
+        <v>582.80399999999997</v>
       </c>
       <c r="F4">
-        <v>576.94299999999998</v>
+        <v>577.21400000000006</v>
       </c>
       <c r="G4">
-        <v>577.78099999999995</v>
+        <v>578</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -6871,19 +6907,19 @@
         <v>555</v>
       </c>
       <c r="C5">
-        <v>620.83000000000004</v>
+        <v>620.70899999999995</v>
       </c>
       <c r="D5">
-        <v>596.31899999999996</v>
+        <v>596.96400000000006</v>
       </c>
       <c r="E5">
-        <v>593.95699999999999</v>
+        <v>594.01800000000003</v>
       </c>
       <c r="F5">
-        <v>585.72299999999996</v>
+        <v>586.18200000000002</v>
       </c>
       <c r="G5">
-        <v>585.38300000000004</v>
+        <v>585.85500000000002</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -6894,19 +6930,19 @@
         <v>555</v>
       </c>
       <c r="C6">
-        <v>600.846</v>
+        <v>599.21500000000003</v>
       </c>
       <c r="D6">
-        <v>594.71799999999996</v>
+        <v>600.97799999999995</v>
       </c>
       <c r="E6">
-        <v>591.48699999999997</v>
+        <v>592.52700000000004</v>
       </c>
       <c r="F6">
-        <v>586.30799999999999</v>
+        <v>587.28</v>
       </c>
       <c r="G6">
-        <v>585.71799999999996</v>
+        <v>586.74199999999996</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -6917,19 +6953,19 @@
         <v>555</v>
       </c>
       <c r="C7">
-        <v>611</v>
+        <v>606.64400000000001</v>
       </c>
       <c r="D7">
-        <v>604.43200000000002</v>
+        <v>603.31100000000004</v>
       </c>
       <c r="E7">
-        <v>656.75699999999995</v>
+        <v>657.84400000000005</v>
       </c>
       <c r="F7">
-        <v>591.97299999999996</v>
+        <v>591.91099999999994</v>
       </c>
       <c r="G7">
-        <v>593.08100000000002</v>
+        <v>593.02200000000005</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -6940,19 +6976,19 @@
         <v>555</v>
       </c>
       <c r="C8">
-        <v>627.72199999999998</v>
+        <v>626.50599999999997</v>
       </c>
       <c r="D8">
-        <v>624</v>
+        <v>621.51900000000001</v>
       </c>
       <c r="E8">
-        <v>639.36099999999999</v>
+        <v>635.84</v>
       </c>
       <c r="F8">
-        <v>602.44399999999996</v>
+        <v>601.27200000000005</v>
       </c>
       <c r="G8">
-        <v>604.11099999999999</v>
+        <v>602.85199999999998</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -6963,19 +6999,19 @@
         <v>555</v>
       </c>
       <c r="C9">
-        <v>612.57100000000003</v>
+        <v>609.60599999999999</v>
       </c>
       <c r="D9">
-        <v>626.17899999999997</v>
+        <v>623.21199999999999</v>
       </c>
       <c r="E9">
-        <v>734.07100000000003</v>
+        <v>739.57600000000002</v>
       </c>
       <c r="F9">
-        <v>613.14300000000003</v>
+        <v>621.303</v>
       </c>
       <c r="G9">
-        <v>608.89300000000003</v>
+        <v>615.48500000000001</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -6986,19 +7022,19 @@
         <v>555</v>
       </c>
       <c r="C10">
-        <v>597.27300000000002</v>
+        <v>595.75</v>
       </c>
       <c r="D10">
-        <v>632.63599999999997</v>
+        <v>631.25</v>
       </c>
       <c r="E10">
-        <v>648.86400000000003</v>
+        <v>643.75</v>
       </c>
       <c r="F10">
-        <v>623.68200000000002</v>
+        <v>620.5</v>
       </c>
       <c r="G10">
-        <v>622.54499999999996</v>
+        <v>619.5</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -7032,19 +7068,19 @@
         <v>555</v>
       </c>
       <c r="C12">
-        <v>591.44399999999996</v>
+        <v>590</v>
       </c>
       <c r="D12">
-        <v>633.66700000000003</v>
+        <v>627.6</v>
       </c>
       <c r="E12">
-        <v>657.44399999999996</v>
+        <v>649.20000000000005</v>
       </c>
       <c r="F12">
-        <v>666.33299999999997</v>
+        <v>657</v>
       </c>
       <c r="G12">
-        <v>649.22199999999998</v>
+        <v>641.6</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -7055,19 +7091,19 @@
         <v>555</v>
       </c>
       <c r="C13">
-        <v>608</v>
+        <v>613.875</v>
       </c>
       <c r="D13">
-        <v>650.83299999999997</v>
+        <v>656.125</v>
       </c>
       <c r="E13">
-        <v>732.5</v>
+        <v>758.75</v>
       </c>
       <c r="F13">
-        <v>632.16700000000003</v>
+        <v>650.125</v>
       </c>
       <c r="G13">
-        <v>632.16700000000003</v>
+        <v>655.625</v>
       </c>
     </row>
     <row r="14" spans="1:7">

</xml_diff>

<commit_message>
Ajout de la partie 'simulations' du rapport
</commit_message>
<xml_diff>
--- a/Simulations/tests/lissage_resultats/donnees.xlsx
+++ b/Simulations/tests/lissage_resultats/donnees.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14480" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14480" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TTFF_alea" sheetId="7" r:id="rId1"/>
@@ -1575,7 +1575,7 @@
         <c:axId val="2047313464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="9000.0"/>
+          <c:max val="2000.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2242,10 +2242,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>TTFF_alea_real!$A$3:$A$13</c:f>
+              <c:f>TTFF_alea_real!$A$3:$A$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0.2</c:v>
                 </c:pt>
@@ -2278,16 +2278,19 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>TTFF_alea_real!$B$3:$B$13</c:f>
+              <c:f>TTFF_alea_real!$B$3:$B$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>555.0</c:v>
                 </c:pt>
@@ -2319,6 +2322,9 @@
                   <c:v>555.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>555.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>555.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2345,10 +2351,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>TTFF_alea_real!$A$3:$A$13</c:f>
+              <c:f>TTFF_alea_real!$A$3:$A$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0.2</c:v>
                 </c:pt>
@@ -2381,18 +2387,21 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>TTFF_alea_real!$C$3:$C$13</c:f>
+              <c:f>TTFF_alea_real!$C$3:$C$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>571.467</c:v>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>570.89</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>573.756</c:v>
@@ -2413,16 +2422,19 @@
                   <c:v>593.633</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>594.667</c:v>
+                  <c:v>597.763</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>593.462</c:v>
+                  <c:v>592.17</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>586.8819999999999</c:v>
+                  <c:v>590.375</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>602.158</c:v>
+                  <c:v>610.862</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>618.167</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2448,10 +2460,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>TTFF_alea_real!$A$3:$A$13</c:f>
+              <c:f>TTFF_alea_real!$A$3:$A$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0.2</c:v>
                 </c:pt>
@@ -2484,18 +2496,21 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>TTFF_alea_real!$D$3:$D$13</c:f>
+              <c:f>TTFF_alea_real!$D$3:$D$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>569.4</c:v>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>568.836</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>572.849</c:v>
@@ -2516,16 +2531,19 @@
                   <c:v>596.468</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>600.074</c:v>
+                  <c:v>601.026</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>596.692</c:v>
+                  <c:v>597.038</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>597.588</c:v>
+                  <c:v>596.438</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>606.579</c:v>
+                  <c:v>613.069</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>627.667</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2551,10 +2569,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>TTFF_alea_real!$A$3:$A$13</c:f>
+              <c:f>TTFF_alea_real!$A$3:$A$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0.2</c:v>
                 </c:pt>
@@ -2587,18 +2605,21 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>TTFF_alea_real!$E$3:$E$13</c:f>
+              <c:f>TTFF_alea_real!$E$3:$E$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>573.7329999999999</c:v>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>573.247</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>575.487</c:v>
@@ -2619,16 +2640,19 @@
                   <c:v>592.975</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>609.074</c:v>
+                  <c:v>605.737</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>600.538</c:v>
+                  <c:v>598.434</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>621.941</c:v>
+                  <c:v>614.562</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>614.789</c:v>
+                  <c:v>631.414</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>623.833</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2654,10 +2678,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>TTFF_alea_real!$A$3:$A$13</c:f>
+              <c:f>TTFF_alea_real!$A$3:$A$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0.2</c:v>
                 </c:pt>
@@ -2690,18 +2714,21 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>TTFF_alea_real!$F$3:$F$13</c:f>
+              <c:f>TTFF_alea_real!$F$3:$F$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>565.367</c:v>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>564.5069999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>567.084</c:v>
@@ -2722,16 +2749,19 @@
                   <c:v>575.886</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>576.222</c:v>
+                  <c:v>577.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>576.769</c:v>
+                  <c:v>578.66</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>576.412</c:v>
+                  <c:v>576.875</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>580.684</c:v>
+                  <c:v>588.241</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>604.167</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2757,10 +2787,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>TTFF_alea_real!$A$3:$A$13</c:f>
+              <c:f>TTFF_alea_real!$A$3:$A$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0.2</c:v>
                 </c:pt>
@@ -2793,18 +2823,21 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>TTFF_alea_real!$G$3:$G$13</c:f>
+              <c:f>TTFF_alea_real!$G$3:$G$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>566.467</c:v>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>565.575</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>568.328</c:v>
@@ -2825,16 +2858,19 @@
                   <c:v>578.848</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>577.889</c:v>
+                  <c:v>578.789</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>579.923</c:v>
+                  <c:v>581.113</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>576.059</c:v>
+                  <c:v>576.938</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>586.263</c:v>
+                  <c:v>591.4829999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>600.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2946,10 +2982,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>PCN_alea_real!$A$2:$A$12</c:f>
+              <c:f>PCN_alea_real!$A$3:$A$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0.2</c:v>
                 </c:pt>
@@ -2982,16 +3018,19 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>PCN_alea_real!$B$2:$B$12</c:f>
+              <c:f>PCN_alea_real!$B$3:$B$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>555.0</c:v>
                 </c:pt>
@@ -3023,6 +3062,9 @@
                   <c:v>555.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>555.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>555.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -3049,10 +3091,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>PCN_alea_real!$A$2:$A$12</c:f>
+              <c:f>PCN_alea_real!$A$3:$A$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0.2</c:v>
                 </c:pt>
@@ -3085,18 +3127,21 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>PCN_alea_real!$C$2:$C$12</c:f>
+              <c:f>PCN_alea_real!$C$3:$C$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>871.2</c:v>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>890.143</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>908.111</c:v>
@@ -3117,16 +3162,19 @@
                   <c:v>920.273</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>963.167</c:v>
+                  <c:v>962.158</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>915.25</c:v>
+                  <c:v>949.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>935.5</c:v>
+                  <c:v>907.364</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>923.0</c:v>
+                  <c:v>893.4</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1019.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3152,10 +3200,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>PCN_alea_real!$A$2:$A$12</c:f>
+              <c:f>PCN_alea_real!$A$3:$A$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0.2</c:v>
                 </c:pt>
@@ -3188,18 +3236,21 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>PCN_alea_real!$D$2:$D$12</c:f>
+              <c:f>PCN_alea_real!$D$3:$D$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>961.6</c:v>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>945.714</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1027.22</c:v>
@@ -3220,16 +3271,19 @@
                   <c:v>988.818</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1009.5</c:v>
+                  <c:v>1021.63</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1017.75</c:v>
+                  <c:v>1019.33</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1015.0</c:v>
+                  <c:v>1012.09</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1051.4</c:v>
+                  <c:v>1014.6</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>961.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3255,10 +3309,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>PCN_alea_real!$A$2:$A$12</c:f>
+              <c:f>PCN_alea_real!$A$3:$A$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0.2</c:v>
                 </c:pt>
@@ -3291,18 +3345,21 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>PCN_alea_real!$E$2:$E$12</c:f>
+              <c:f>PCN_alea_real!$E$3:$E$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>3365.8</c:v>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>3224.71</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>3079.11</c:v>
@@ -3323,16 +3380,19 @@
                   <c:v>3397.91</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3579.5</c:v>
+                  <c:v>3748.79</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3676.5</c:v>
+                  <c:v>3708.83</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3291.5</c:v>
+                  <c:v>3688.82</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4528.6</c:v>
+                  <c:v>4088.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3601.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3358,10 +3418,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>PCN_alea_real!$A$2:$A$12</c:f>
+              <c:f>PCN_alea_real!$A$3:$A$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0.2</c:v>
                 </c:pt>
@@ -3394,18 +3454,21 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>PCN_alea_real!$F$2:$F$12</c:f>
+              <c:f>PCN_alea_real!$F$3:$F$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>1426.6</c:v>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1439.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1427.56</c:v>
@@ -3426,16 +3489,19 @@
                   <c:v>1250.45</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1356.0</c:v>
+                  <c:v>1370.16</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1401.5</c:v>
+                  <c:v>1434.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1359.5</c:v>
+                  <c:v>1457.73</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1755.4</c:v>
+                  <c:v>1594.2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1431.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3461,10 +3527,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>PCN_alea_real!$A$2:$A$12</c:f>
+              <c:f>PCN_alea_real!$A$3:$A$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0.2</c:v>
                 </c:pt>
@@ -3497,18 +3563,21 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>PCN_alea_real!$G$2:$G$12</c:f>
+              <c:f>PCN_alea_real!$G$3:$G$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>1601.4</c:v>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1638.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1651.11</c:v>
@@ -3529,16 +3598,19 @@
                   <c:v>1425.36</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1474.0</c:v>
+                  <c:v>1498.16</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1484.5</c:v>
+                  <c:v>1503.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1682.5</c:v>
+                  <c:v>1648.45</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2076.2</c:v>
+                  <c:v>1801.8</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1624.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3649,52 +3721,64 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>LC_alea_real!$A$3:$A$13</c:f>
+              <c:f>LC_alea_real!$A$2:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>0.2</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>0.25</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>0.3</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>0.35</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>0.4</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>0.45</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>0.5</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>0.55</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>0.6</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>0.65</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.85</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>LC_alea_real!$B$3:$B$13</c:f>
+              <c:f>LC_alea_real!$B$2:$B$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>555.0</c:v>
                 </c:pt>
@@ -3726,6 +3810,18 @@
                   <c:v>555.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>555.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>555.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>555.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>555.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>555.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -3752,84 +3848,108 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>LC_alea_real!$A$3:$A$13</c:f>
+              <c:f>LC_alea_real!$A$2:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>0.2</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>0.25</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>0.3</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>0.35</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>0.4</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>0.45</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>0.5</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>0.55</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>0.6</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>0.65</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.85</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>LC_alea_real!$C$3:$C$13</c:f>
+              <c:f>LC_alea_real!$C$2:$C$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>603.966</c:v>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>625.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>607.857</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>633.768</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>620.709</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>599.215</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>606.644</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>626.506</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>609.606</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>595.75</c:v>
-                </c:pt>
                 <c:pt idx="8">
-                  <c:v>596.1</c:v>
+                  <c:v>611.029</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>590.0</c:v>
+                  <c:v>641.444</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>613.875</c:v>
+                  <c:v>597.917</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>609.957</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>605.571</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>597.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>635.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3855,84 +3975,108 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>LC_alea_real!$A$3:$A$13</c:f>
+              <c:f>LC_alea_real!$A$2:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>0.2</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>0.25</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>0.3</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>0.35</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>0.4</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>0.45</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>0.5</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>0.55</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>0.6</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>0.65</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.85</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>LC_alea_real!$D$3:$D$13</c:f>
+              <c:f>LC_alea_real!$D$2:$D$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>580.414</c:v>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>577.4</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>579.343</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>585.589</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>596.9640000000001</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>600.978</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>603.311</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>621.519</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>623.212</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>631.25</c:v>
-                </c:pt>
                 <c:pt idx="8">
-                  <c:v>622.1</c:v>
+                  <c:v>629.4640000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>627.6</c:v>
+                  <c:v>635.489</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>656.125</c:v>
+                  <c:v>632.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>670.739</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>645.571</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>614.333</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>599.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3958,84 +4102,108 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>LC_alea_real!$A$3:$A$13</c:f>
+              <c:f>LC_alea_real!$A$2:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>0.2</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>0.25</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>0.3</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>0.35</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>0.4</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>0.45</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>0.5</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>0.55</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>0.6</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>0.65</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.85</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>LC_alea_real!$E$3:$E$13</c:f>
+              <c:f>LC_alea_real!$E$2:$E$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>577.069</c:v>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>590.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>575.943</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>582.804</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>594.018</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>592.527</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>657.8440000000001</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>635.84</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>739.576</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>643.75</c:v>
-                </c:pt>
                 <c:pt idx="8">
-                  <c:v>674.6</c:v>
+                  <c:v>737.812</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>649.2</c:v>
+                  <c:v>689.178</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>758.75</c:v>
+                  <c:v>638.583</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1046.3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>627.286</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>884.333</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>635.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4061,84 +4229,108 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>LC_alea_real!$A$3:$A$13</c:f>
+              <c:f>LC_alea_real!$A$2:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>0.2</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>0.25</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>0.3</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>0.35</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>0.4</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>0.45</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>0.5</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>0.55</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>0.6</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>0.65</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.85</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>LC_alea_real!$F$3:$F$13</c:f>
+              <c:f>LC_alea_real!$F$2:$F$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>573.379</c:v>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>597.8</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>572.457</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>577.214</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>586.182</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>587.28</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>591.9109999999999</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>601.272</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>621.303</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>620.5</c:v>
-                </c:pt>
                 <c:pt idx="8">
-                  <c:v>613.0</c:v>
+                  <c:v>622.159</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>657.0</c:v>
+                  <c:v>614.956</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>650.125</c:v>
+                  <c:v>635.333</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>670.478</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>624.714</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>602.333</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>633.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4164,84 +4356,108 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>LC_alea_real!$A$3:$A$13</c:f>
+              <c:f>LC_alea_real!$A$2:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>0.2</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>0.25</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>0.3</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>0.35</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>0.4</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>0.45</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>0.5</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>0.55</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>0.6</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>0.65</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.85</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>LC_alea_real!$G$3:$G$13</c:f>
+              <c:f>LC_alea_real!$G$2:$G$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>573.897</c:v>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>590.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>572.886</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>578.0</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>585.855</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>586.742</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>593.022</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>602.852</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>615.485</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>619.5</c:v>
-                </c:pt>
                 <c:pt idx="8">
-                  <c:v>612.8</c:v>
+                  <c:v>621.609</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>641.6</c:v>
+                  <c:v>614.378</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>655.625</c:v>
+                  <c:v>628.417</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>684.826</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>624.714</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>602.333</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>629.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5326,8 +5542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6009,7 +6225,7 @@
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6042,19 +6258,19 @@
         <v>555</v>
       </c>
       <c r="C2">
-        <v>573.66700000000003</v>
+        <v>570.6</v>
       </c>
       <c r="D2">
-        <v>571.66700000000003</v>
+        <v>568.6</v>
       </c>
       <c r="E2">
-        <v>579</v>
+        <v>584.6</v>
       </c>
       <c r="F2">
-        <v>573.66700000000003</v>
+        <v>573.4</v>
       </c>
       <c r="G2">
-        <v>576.33299999999997</v>
+        <v>575.79999999999995</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -6065,19 +6281,19 @@
         <v>555</v>
       </c>
       <c r="C3">
-        <v>571.46699999999998</v>
+        <v>570.89</v>
       </c>
       <c r="D3">
-        <v>569.4</v>
+        <v>568.83600000000001</v>
       </c>
       <c r="E3">
-        <v>573.73299999999995</v>
+        <v>573.24699999999996</v>
       </c>
       <c r="F3">
-        <v>565.36699999999996</v>
+        <v>564.50699999999995</v>
       </c>
       <c r="G3">
-        <v>566.46699999999998</v>
+        <v>565.57500000000005</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -6226,19 +6442,19 @@
         <v>555</v>
       </c>
       <c r="C10">
-        <v>594.66700000000003</v>
+        <v>597.76300000000003</v>
       </c>
       <c r="D10">
-        <v>600.07399999999996</v>
+        <v>601.02599999999995</v>
       </c>
       <c r="E10">
-        <v>609.07399999999996</v>
+        <v>605.73699999999997</v>
       </c>
       <c r="F10">
-        <v>576.22199999999998</v>
+        <v>577.5</v>
       </c>
       <c r="G10">
-        <v>577.88900000000001</v>
+        <v>578.78899999999999</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -6249,19 +6465,19 @@
         <v>555</v>
       </c>
       <c r="C11">
-        <v>593.46199999999999</v>
+        <v>592.16999999999996</v>
       </c>
       <c r="D11">
-        <v>596.69200000000001</v>
+        <v>597.03800000000001</v>
       </c>
       <c r="E11">
-        <v>600.53800000000001</v>
+        <v>598.43399999999997</v>
       </c>
       <c r="F11">
-        <v>576.76900000000001</v>
+        <v>578.66</v>
       </c>
       <c r="G11">
-        <v>579.923</v>
+        <v>581.11300000000006</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -6272,19 +6488,19 @@
         <v>555</v>
       </c>
       <c r="C12">
-        <v>586.88199999999995</v>
+        <v>590.375</v>
       </c>
       <c r="D12">
-        <v>597.58799999999997</v>
+        <v>596.43799999999999</v>
       </c>
       <c r="E12">
-        <v>621.94100000000003</v>
+        <v>614.56200000000001</v>
       </c>
       <c r="F12">
-        <v>576.41200000000003</v>
+        <v>576.875</v>
       </c>
       <c r="G12">
-        <v>576.05899999999997</v>
+        <v>576.93799999999999</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -6295,19 +6511,19 @@
         <v>555</v>
       </c>
       <c r="C13">
-        <v>602.15800000000002</v>
+        <v>610.86199999999997</v>
       </c>
       <c r="D13">
-        <v>606.57899999999995</v>
+        <v>613.06899999999996</v>
       </c>
       <c r="E13">
-        <v>614.78899999999999</v>
+        <v>631.41399999999999</v>
       </c>
       <c r="F13">
-        <v>580.68399999999997</v>
+        <v>588.24099999999999</v>
       </c>
       <c r="G13">
-        <v>586.26300000000003</v>
+        <v>591.48299999999995</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -6318,19 +6534,19 @@
         <v>555</v>
       </c>
       <c r="C14">
-        <v>648.33299999999997</v>
+        <v>618.16700000000003</v>
       </c>
       <c r="D14">
-        <v>669.33299999999997</v>
+        <v>627.66700000000003</v>
       </c>
       <c r="E14">
-        <v>621.66700000000003</v>
+        <v>623.83299999999997</v>
       </c>
       <c r="F14">
-        <v>616</v>
+        <v>604.16700000000003</v>
       </c>
       <c r="G14">
-        <v>608</v>
+        <v>600</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -6341,85 +6557,131 @@
         <v>555</v>
       </c>
       <c r="C15">
-        <v>649</v>
+        <v>611.5</v>
       </c>
       <c r="D15">
-        <v>647</v>
+        <v>614.5</v>
       </c>
       <c r="E15">
-        <v>639</v>
+        <v>613.5</v>
       </c>
       <c r="F15">
-        <v>614</v>
+        <v>592</v>
       </c>
       <c r="G15">
-        <v>604</v>
+        <v>587.5</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16">
-        <v>0.9</v>
+        <v>0.85</v>
       </c>
       <c r="B16">
         <v>555</v>
       </c>
       <c r="C16">
+        <v>611</v>
+      </c>
+      <c r="D16">
+        <v>609</v>
+      </c>
+      <c r="E16">
+        <v>737</v>
+      </c>
+      <c r="F16">
+        <v>583</v>
+      </c>
+      <c r="G16">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17">
+        <v>0.9</v>
+      </c>
+      <c r="B17">
+        <v>555</v>
+      </c>
+      <c r="C17">
         <v>573</v>
       </c>
-      <c r="D16">
+      <c r="D17">
         <v>571</v>
       </c>
-      <c r="E16">
+      <c r="E17">
         <v>573</v>
       </c>
-      <c r="F16">
+      <c r="F17">
         <v>571</v>
       </c>
-      <c r="G16">
+      <c r="G17">
         <v>571</v>
       </c>
     </row>
-    <row r="24" spans="1:1">
+    <row r="18" spans="1:7">
+      <c r="A18">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B18">
+        <v>555</v>
+      </c>
+      <c r="C18">
+        <v>587</v>
+      </c>
+      <c r="D18">
+        <v>585</v>
+      </c>
+      <c r="E18">
+        <v>587</v>
+      </c>
+      <c r="F18">
+        <v>585</v>
+      </c>
+      <c r="G18">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:7">
       <c r="A25" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:1">
+    <row r="26" spans="1:7">
       <c r="A26" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:1">
+    <row r="27" spans="1:7">
       <c r="A27" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:7">
       <c r="A28" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:1">
+    <row r="29" spans="1:7">
       <c r="A29" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:1">
+    <row r="30" spans="1:7">
       <c r="A30" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:1">
+    <row r="31" spans="1:7">
       <c r="A31" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:1">
+    <row r="32" spans="1:7">
       <c r="A32" t="s">
         <v>14</v>
       </c>
@@ -6438,7 +6700,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -6468,323 +6730,346 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="B2">
         <v>555</v>
       </c>
       <c r="C2">
-        <v>871.2</v>
+        <v>803</v>
       </c>
       <c r="D2">
-        <v>961.6</v>
+        <v>899</v>
       </c>
       <c r="E2">
-        <v>3365.8</v>
+        <v>2521</v>
       </c>
       <c r="F2">
-        <v>1426.6</v>
+        <v>1109</v>
       </c>
       <c r="G2">
-        <v>1601.4</v>
+        <v>969</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3">
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
       <c r="B3">
         <v>555</v>
       </c>
       <c r="C3">
-        <v>908.11099999999999</v>
+        <v>890.14300000000003</v>
       </c>
       <c r="D3">
-        <v>1027.22</v>
+        <v>945.71400000000006</v>
       </c>
       <c r="E3">
-        <v>3079.11</v>
+        <v>3224.71</v>
       </c>
       <c r="F3">
-        <v>1427.56</v>
+        <v>1439</v>
       </c>
       <c r="G3">
-        <v>1651.11</v>
+        <v>1638</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4">
-        <v>0.3</v>
+        <v>0.25</v>
       </c>
       <c r="B4">
         <v>555</v>
       </c>
       <c r="C4">
-        <v>995.66700000000003</v>
+        <v>908.11099999999999</v>
       </c>
       <c r="D4">
-        <v>995.22199999999998</v>
+        <v>1027.22</v>
       </c>
       <c r="E4">
-        <v>2843.67</v>
+        <v>3079.11</v>
       </c>
       <c r="F4">
-        <v>1260.78</v>
+        <v>1427.56</v>
       </c>
       <c r="G4">
-        <v>1458.11</v>
+        <v>1651.11</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5">
-        <v>0.35</v>
+        <v>0.3</v>
       </c>
       <c r="B5">
         <v>555</v>
       </c>
       <c r="C5">
-        <v>904.42899999999997</v>
+        <v>995.66700000000003</v>
       </c>
       <c r="D5">
-        <v>1111</v>
+        <v>995.22199999999998</v>
       </c>
       <c r="E5">
-        <v>3271</v>
+        <v>2843.67</v>
       </c>
       <c r="F5">
-        <v>1394.14</v>
+        <v>1260.78</v>
       </c>
       <c r="G5">
-        <v>1649</v>
+        <v>1458.11</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6">
-        <v>0.4</v>
+        <v>0.35</v>
       </c>
       <c r="B6">
         <v>555</v>
       </c>
       <c r="C6">
-        <v>918.71400000000006</v>
+        <v>904.42899999999997</v>
       </c>
       <c r="D6">
-        <v>1001</v>
+        <v>1111</v>
       </c>
       <c r="E6">
-        <v>3351.57</v>
+        <v>3271</v>
       </c>
       <c r="F6">
-        <v>1232.43</v>
+        <v>1394.14</v>
       </c>
       <c r="G6">
-        <v>1331.29</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7">
-        <v>0.45</v>
+        <v>0.4</v>
       </c>
       <c r="B7">
         <v>555</v>
       </c>
       <c r="C7">
-        <v>926.42899999999997</v>
+        <v>918.71400000000006</v>
       </c>
       <c r="D7">
-        <v>1013</v>
+        <v>1001</v>
       </c>
       <c r="E7">
-        <v>3632.86</v>
+        <v>3351.57</v>
       </c>
       <c r="F7">
-        <v>1333.43</v>
+        <v>1232.43</v>
       </c>
       <c r="G7">
-        <v>1423</v>
+        <v>1331.29</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8">
-        <v>0.5</v>
+        <v>0.45</v>
       </c>
       <c r="B8">
         <v>555</v>
       </c>
       <c r="C8">
-        <v>920.27300000000002</v>
+        <v>926.42899999999997</v>
       </c>
       <c r="D8">
-        <v>988.81799999999998</v>
+        <v>1013</v>
       </c>
       <c r="E8">
-        <v>3397.91</v>
+        <v>3632.86</v>
       </c>
       <c r="F8">
-        <v>1250.45</v>
+        <v>1333.43</v>
       </c>
       <c r="G8">
-        <v>1425.36</v>
+        <v>1423</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9">
-        <v>0.55000000000000004</v>
+        <v>0.5</v>
       </c>
       <c r="B9">
         <v>555</v>
       </c>
       <c r="C9">
-        <v>963.16700000000003</v>
+        <v>920.27300000000002</v>
       </c>
       <c r="D9">
-        <v>1009.5</v>
+        <v>988.81799999999998</v>
       </c>
       <c r="E9">
-        <v>3579.5</v>
+        <v>3397.91</v>
       </c>
       <c r="F9">
-        <v>1356</v>
+        <v>1250.45</v>
       </c>
       <c r="G9">
-        <v>1474</v>
+        <v>1425.36</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10">
-        <v>0.6</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="B10">
         <v>555</v>
       </c>
       <c r="C10">
-        <v>915.25</v>
+        <v>962.15800000000002</v>
       </c>
       <c r="D10">
-        <v>1017.75</v>
+        <v>1021.63</v>
       </c>
       <c r="E10">
-        <v>3676.5</v>
+        <v>3748.79</v>
       </c>
       <c r="F10">
-        <v>1401.5</v>
+        <v>1370.16</v>
       </c>
       <c r="G10">
-        <v>1484.5</v>
+        <v>1498.16</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11">
-        <v>0.65</v>
+        <v>0.6</v>
       </c>
       <c r="B11">
         <v>555</v>
       </c>
       <c r="C11">
-        <v>935.5</v>
+        <v>949</v>
       </c>
       <c r="D11">
-        <v>1015</v>
+        <v>1019.33</v>
       </c>
       <c r="E11">
-        <v>3291.5</v>
+        <v>3708.83</v>
       </c>
       <c r="F11">
-        <v>1359.5</v>
+        <v>1434</v>
       </c>
       <c r="G11">
-        <v>1682.5</v>
+        <v>1503.5</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12">
-        <v>0.7</v>
+        <v>0.65</v>
       </c>
       <c r="B12">
         <v>555</v>
       </c>
       <c r="C12">
-        <v>923</v>
+        <v>907.36400000000003</v>
       </c>
       <c r="D12">
-        <v>1051.4000000000001</v>
+        <v>1012.09</v>
       </c>
       <c r="E12">
-        <v>4528.6000000000004</v>
+        <v>3688.82</v>
       </c>
       <c r="F12">
-        <v>1755.4</v>
+        <v>1457.73</v>
       </c>
       <c r="G12">
-        <v>2076.1999999999998</v>
+        <v>1648.45</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13">
-        <v>0.75</v>
+        <v>0.7</v>
       </c>
       <c r="B13">
         <v>555</v>
       </c>
       <c r="C13">
-        <v>987</v>
+        <v>893.4</v>
       </c>
       <c r="D13">
-        <v>959</v>
+        <v>1014.6</v>
       </c>
       <c r="E13">
-        <v>3351</v>
+        <v>4088</v>
       </c>
       <c r="F13">
-        <v>1273</v>
+        <v>1594.2</v>
       </c>
       <c r="G13">
-        <v>1243</v>
+        <v>1801.8</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14">
-        <v>0.8</v>
+        <v>0.75</v>
       </c>
       <c r="B14">
         <v>555</v>
       </c>
       <c r="C14">
-        <v>1033</v>
+        <v>1019</v>
       </c>
       <c r="D14">
-        <v>885</v>
+        <v>961</v>
       </c>
       <c r="E14">
-        <v>3089</v>
+        <v>3601</v>
       </c>
       <c r="F14">
-        <v>1175</v>
+        <v>1431</v>
       </c>
       <c r="G14">
-        <v>1341</v>
+        <v>1624</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="B15">
         <v>555</v>
       </c>
       <c r="C15">
+        <v>1177</v>
+      </c>
+      <c r="D15">
+        <v>959</v>
+      </c>
+      <c r="E15">
+        <v>3869</v>
+      </c>
+      <c r="F15">
+        <v>1268</v>
+      </c>
+      <c r="G15">
+        <v>1414</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16">
+        <v>0.9</v>
+      </c>
+      <c r="B16">
+        <v>555</v>
+      </c>
+      <c r="C16">
         <v>952</v>
       </c>
-      <c r="D15">
+      <c r="D16">
         <v>1045</v>
       </c>
-      <c r="E15">
+      <c r="E16">
         <v>5008</v>
       </c>
-      <c r="F15">
+      <c r="F16">
         <v>1772</v>
       </c>
-      <c r="G15">
+      <c r="G16">
         <v>1943</v>
       </c>
     </row>
@@ -6802,10 +7087,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6838,19 +7123,19 @@
         <v>555</v>
       </c>
       <c r="C2">
-        <v>582.33299999999997</v>
+        <v>625</v>
       </c>
       <c r="D2">
-        <v>577</v>
+        <v>577.4</v>
       </c>
       <c r="E2">
-        <v>579</v>
+        <v>590.6</v>
       </c>
       <c r="F2">
-        <v>577</v>
+        <v>597.79999999999995</v>
       </c>
       <c r="G2">
-        <v>577</v>
+        <v>590.6</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -6861,19 +7146,19 @@
         <v>555</v>
       </c>
       <c r="C3">
-        <v>603.96600000000001</v>
+        <v>607.85699999999997</v>
       </c>
       <c r="D3">
-        <v>580.41399999999999</v>
+        <v>579.34299999999996</v>
       </c>
       <c r="E3">
-        <v>577.06899999999996</v>
+        <v>575.94299999999998</v>
       </c>
       <c r="F3">
-        <v>573.37900000000002</v>
+        <v>572.45699999999999</v>
       </c>
       <c r="G3">
-        <v>573.89700000000005</v>
+        <v>572.88599999999997</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -7022,19 +7307,19 @@
         <v>555</v>
       </c>
       <c r="C10">
-        <v>595.75</v>
+        <v>611.029</v>
       </c>
       <c r="D10">
-        <v>631.25</v>
+        <v>629.46400000000006</v>
       </c>
       <c r="E10">
-        <v>643.75</v>
+        <v>737.81200000000001</v>
       </c>
       <c r="F10">
-        <v>620.5</v>
+        <v>622.15899999999999</v>
       </c>
       <c r="G10">
-        <v>619.5</v>
+        <v>621.60900000000004</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -7045,19 +7330,19 @@
         <v>555</v>
       </c>
       <c r="C11">
-        <v>596.1</v>
+        <v>641.44399999999996</v>
       </c>
       <c r="D11">
-        <v>622.1</v>
+        <v>635.48900000000003</v>
       </c>
       <c r="E11">
-        <v>674.6</v>
+        <v>689.178</v>
       </c>
       <c r="F11">
-        <v>613</v>
+        <v>614.95600000000002</v>
       </c>
       <c r="G11">
-        <v>612.79999999999995</v>
+        <v>614.37800000000004</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -7068,19 +7353,19 @@
         <v>555</v>
       </c>
       <c r="C12">
-        <v>590</v>
+        <v>597.91700000000003</v>
       </c>
       <c r="D12">
-        <v>627.6</v>
+        <v>632.5</v>
       </c>
       <c r="E12">
-        <v>649.20000000000005</v>
+        <v>638.58299999999997</v>
       </c>
       <c r="F12">
-        <v>657</v>
+        <v>635.33299999999997</v>
       </c>
       <c r="G12">
-        <v>641.6</v>
+        <v>628.41700000000003</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -7091,19 +7376,19 @@
         <v>555</v>
       </c>
       <c r="C13">
-        <v>613.875</v>
+        <v>609.95699999999999</v>
       </c>
       <c r="D13">
-        <v>656.125</v>
+        <v>670.73900000000003</v>
       </c>
       <c r="E13">
-        <v>758.75</v>
+        <v>1046.3</v>
       </c>
       <c r="F13">
-        <v>650.125</v>
+        <v>670.47799999999995</v>
       </c>
       <c r="G13">
-        <v>655.625</v>
+        <v>684.82600000000002</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -7114,19 +7399,19 @@
         <v>555</v>
       </c>
       <c r="C14">
-        <v>597</v>
+        <v>605.57100000000003</v>
       </c>
       <c r="D14">
-        <v>681.66700000000003</v>
+        <v>645.57100000000003</v>
       </c>
       <c r="E14">
-        <v>658.33299999999997</v>
+        <v>627.28599999999994</v>
       </c>
       <c r="F14">
-        <v>655</v>
+        <v>624.71400000000006</v>
       </c>
       <c r="G14">
-        <v>655</v>
+        <v>624.71400000000006</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -7137,42 +7422,88 @@
         <v>555</v>
       </c>
       <c r="C15">
-        <v>567</v>
+        <v>597</v>
       </c>
       <c r="D15">
-        <v>679</v>
+        <v>614.33299999999997</v>
       </c>
       <c r="E15">
-        <v>681</v>
+        <v>884.33299999999997</v>
       </c>
       <c r="F15">
-        <v>653</v>
+        <v>602.33299999999997</v>
       </c>
       <c r="G15">
-        <v>653</v>
+        <v>602.33299999999997</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16">
-        <v>0.9</v>
+        <v>0.85</v>
       </c>
       <c r="B16">
         <v>555</v>
       </c>
       <c r="C16">
+        <v>635</v>
+      </c>
+      <c r="D16">
+        <v>599</v>
+      </c>
+      <c r="E16">
+        <v>635</v>
+      </c>
+      <c r="F16">
+        <v>633</v>
+      </c>
+      <c r="G16">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17">
+        <v>0.9</v>
+      </c>
+      <c r="B17">
+        <v>555</v>
+      </c>
+      <c r="C17">
         <v>626</v>
       </c>
-      <c r="D16">
+      <c r="D17">
         <v>571</v>
       </c>
-      <c r="E16">
+      <c r="E17">
         <v>573</v>
       </c>
-      <c r="F16">
+      <c r="F17">
         <v>571</v>
       </c>
-      <c r="G16">
+      <c r="G17">
         <v>571</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B18">
+        <v>555</v>
+      </c>
+      <c r="C18">
+        <v>595</v>
+      </c>
+      <c r="D18">
+        <v>585</v>
+      </c>
+      <c r="E18">
+        <v>587</v>
+      </c>
+      <c r="F18">
+        <v>585</v>
+      </c>
+      <c r="G18">
+        <v>585</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Courbes finales dans excel
</commit_message>
<xml_diff>
--- a/Simulations/tests/lissage_resultats/donnees.xlsx
+++ b/Simulations/tests/lissage_resultats/donnees.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14480" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14480" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="TTFF_alea" sheetId="7" r:id="rId1"/>
@@ -380,7 +380,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>TTFF_alea!$A$2:$A$11</c:f>
+              <c:f>TTFF_alea!$A$3:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -419,7 +419,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>TTFF_alea!$B$2:$B$11</c:f>
+              <c:f>TTFF_alea!$B$3:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -477,7 +477,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>TTFF_alea!$A$2:$A$11</c:f>
+              <c:f>TTFF_alea!$A$3:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -516,39 +516,39 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>TTFF_alea!$C$2:$C$11</c:f>
+              <c:f>TTFF_alea!$C$3:$C$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>466.9</c:v>
+                  <c:v>465.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>468.379</c:v>
+                  <c:v>466.771</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>468.038</c:v>
+                  <c:v>468.353</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>469.909</c:v>
+                  <c:v>469.557</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>474.667</c:v>
+                  <c:v>474.656</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>483.182</c:v>
+                  <c:v>484.768</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>481.885</c:v>
+                  <c:v>481.092</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>486.379</c:v>
+                  <c:v>486.939</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>493.512</c:v>
+                  <c:v>492.733</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>510.486</c:v>
+                  <c:v>509.718</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -574,7 +574,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>TTFF_alea!$A$2:$A$11</c:f>
+              <c:f>TTFF_alea!$A$3:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -613,39 +613,39 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>TTFF_alea!$D$2:$D$11</c:f>
+              <c:f>TTFF_alea!$D$3:$D$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>466.4</c:v>
+                  <c:v>464.481</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>467.241</c:v>
+                  <c:v>465.514</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>467.506</c:v>
+                  <c:v>468.118</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>468.455</c:v>
+                  <c:v>467.969</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>474.444</c:v>
+                  <c:v>474.656</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>483.982</c:v>
+                  <c:v>485.348</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>482.462</c:v>
+                  <c:v>483.092</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>490.448</c:v>
+                  <c:v>490.636</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>499.326</c:v>
+                  <c:v>498.2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>512.943</c:v>
+                  <c:v>511.667</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -671,7 +671,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>TTFF_alea!$A$2:$A$11</c:f>
+              <c:f>TTFF_alea!$A$3:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -710,39 +710,39 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>TTFF_alea!$E$2:$E$11</c:f>
+              <c:f>TTFF_alea!$E$3:$E$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>476.5</c:v>
+                  <c:v>476.481</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>483.172</c:v>
+                  <c:v>480.029</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>485.81</c:v>
+                  <c:v>485.706</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>490.303</c:v>
+                  <c:v>489.454</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>497.778</c:v>
+                  <c:v>497.656</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>497.618</c:v>
+                  <c:v>500.449</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>508.769</c:v>
+                  <c:v>505.646</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>510.241</c:v>
+                  <c:v>510.576</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>518.535</c:v>
+                  <c:v>518.956</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>541.571</c:v>
+                  <c:v>541.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -768,7 +768,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>TTFF_alea!$A$2:$A$11</c:f>
+              <c:f>TTFF_alea!$A$3:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -807,39 +807,39 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>TTFF_alea!$F$2:$F$11</c:f>
+              <c:f>TTFF_alea!$F$3:$F$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>473.8</c:v>
+                  <c:v>476.259</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>476.448</c:v>
+                  <c:v>475.571</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>475.43</c:v>
+                  <c:v>475.196</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>474.364</c:v>
+                  <c:v>474.856</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>484.167</c:v>
+                  <c:v>481.594</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>481.364</c:v>
+                  <c:v>482.507</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>481.692</c:v>
+                  <c:v>481.369</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>483.552</c:v>
+                  <c:v>484.758</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>492.628</c:v>
+                  <c:v>491.178</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>497.857</c:v>
+                  <c:v>498.128</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -865,7 +865,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>TTFF_alea!$A$2:$A$11</c:f>
+              <c:f>TTFF_alea!$A$3:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -904,39 +904,39 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>TTFF_alea!$G$2:$G$11</c:f>
+              <c:f>TTFF_alea!$G$3:$G$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>475.4</c:v>
+                  <c:v>476.926</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>478.069</c:v>
+                  <c:v>477.171</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>476.899</c:v>
+                  <c:v>476.706</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>476.152</c:v>
+                  <c:v>476.237</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>486.778</c:v>
+                  <c:v>483.344</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>483.473</c:v>
+                  <c:v>484.768</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>484.615</c:v>
+                  <c:v>484.046</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>485.069</c:v>
+                  <c:v>486.333</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>495.14</c:v>
+                  <c:v>493.578</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>499.514</c:v>
+                  <c:v>499.359</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -953,21 +953,40 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2047244040"/>
-        <c:axId val="2047247176"/>
+        <c:axId val="2097816376"/>
+        <c:axId val="2097819512"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2047244040"/>
+        <c:axId val="2097816376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR"/>
+                  <a:t>Densité du graphe</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2047247176"/>
+        <c:crossAx val="2097819512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -975,20 +994,43 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2047247176"/>
+        <c:axId val="2097819512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="540.0"/>
           <c:min val="440.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR"/>
+                  <a:t>Time</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="fr-FR" baseline="0"/>
+                  <a:t> To First Fall</a:t>
+                </a:r>
+                <a:endParaRPr lang="fr-FR"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2047244040"/>
+        <c:crossAx val="2097816376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1049,10 +1091,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>PCN_alea!$A$2:$A$9</c:f>
+              <c:f>PCN_alea!$A$2:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>0.15</c:v>
                 </c:pt>
@@ -1076,16 +1118,19 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.55</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>PCN_alea!$B$2:$B$9</c:f>
+              <c:f>PCN_alea!$B$2:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>447.0</c:v>
                 </c:pt>
@@ -1108,6 +1153,9 @@
                   <c:v>447.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>447.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>447.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1134,10 +1182,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>PCN_alea!$A$2:$A$9</c:f>
+              <c:f>PCN_alea!$A$2:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>0.15</c:v>
                 </c:pt>
@@ -1161,39 +1209,45 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.55</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>PCN_alea!$C$2:$C$9</c:f>
+              <c:f>PCN_alea!$C$2:$C$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>949.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1108.0</c:v>
+                  <c:v>1063.57</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1085.33</c:v>
+                  <c:v>1080.86</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1063.18</c:v>
+                  <c:v>1054.29</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1033.86</c:v>
+                  <c:v>1013.26</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1152.54</c:v>
+                  <c:v>1132.76</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1103.6</c:v>
+                  <c:v>1077.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1203.0</c:v>
+                  <c:v>1061.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>965.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1219,10 +1273,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>PCN_alea!$A$2:$A$9</c:f>
+              <c:f>PCN_alea!$A$2:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>0.15</c:v>
                 </c:pt>
@@ -1246,39 +1300,45 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.55</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>PCN_alea!$D$2:$D$9</c:f>
+              <c:f>PCN_alea!$D$2:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>1053.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1109.0</c:v>
+                  <c:v>1072.71</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1244.0</c:v>
+                  <c:v>1298.71</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1325.45</c:v>
+                  <c:v>1342.14</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1534.81</c:v>
+                  <c:v>1456.48</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1301.0</c:v>
+                  <c:v>1378.53</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1288.4</c:v>
+                  <c:v>1330.08</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1839.0</c:v>
+                  <c:v>1558.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1363.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1304,10 +1364,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>PCN_alea!$A$2:$A$9</c:f>
+              <c:f>PCN_alea!$A$2:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>0.15</c:v>
                 </c:pt>
@@ -1331,39 +1391,45 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.55</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>PCN_alea!$E$2:$E$9</c:f>
+              <c:f>PCN_alea!$E$2:$E$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>4385.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4905.33</c:v>
+                  <c:v>4822.14</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5448.83</c:v>
+                  <c:v>5447.71</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5559.45</c:v>
+                  <c:v>5604.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6630.33</c:v>
+                  <c:v>6801.26</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6235.0</c:v>
+                  <c:v>6443.94</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6672.6</c:v>
+                  <c:v>6788.38</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9254.0</c:v>
+                  <c:v>8281.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6199.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1389,10 +1455,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>PCN_alea!$A$2:$A$9</c:f>
+              <c:f>PCN_alea!$A$2:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>0.15</c:v>
                 </c:pt>
@@ -1416,39 +1482,45 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.55</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>PCN_alea!$F$2:$F$9</c:f>
+              <c:f>PCN_alea!$F$2:$F$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>1091.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1222.33</c:v>
+                  <c:v>1317.86</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1470.33</c:v>
+                  <c:v>1474.43</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1294.0</c:v>
+                  <c:v>1311.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1411.57</c:v>
+                  <c:v>1401.65</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1285.46</c:v>
+                  <c:v>1340.29</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1157.8</c:v>
+                  <c:v>1181.15</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1304.0</c:v>
+                  <c:v>1219.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1410.33</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1474,10 +1546,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>PCN_alea!$A$2:$A$9</c:f>
+              <c:f>PCN_alea!$A$2:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>0.15</c:v>
                 </c:pt>
@@ -1501,39 +1573,45 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.55</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>PCN_alea!$G$2:$G$9</c:f>
+              <c:f>PCN_alea!$G$2:$G$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>1219.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1433.0</c:v>
+                  <c:v>1561.57</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1619.17</c:v>
+                  <c:v>1622.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1417.27</c:v>
+                  <c:v>1421.86</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1661.19</c:v>
+                  <c:v>1579.97</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1382.85</c:v>
+                  <c:v>1489.12</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1508.6</c:v>
+                  <c:v>1448.23</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1525.0</c:v>
+                  <c:v>1323.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1601.67</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1550,21 +1628,40 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2047310328"/>
-        <c:axId val="2047313464"/>
+        <c:axId val="2097934376"/>
+        <c:axId val="2097937512"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2047310328"/>
+        <c:axId val="2097934376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR"/>
+                  <a:t>Densité du graphe</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2047313464"/>
+        <c:crossAx val="2097937512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1572,19 +1669,39 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2047313464"/>
+        <c:axId val="2097937512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2000.0"/>
+          <c:min val="400.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR"/>
+                  <a:t>PCN : time to 25% fall</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2047310328"/>
+        <c:crossAx val="2097934376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1645,10 +1762,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>LC_alea!$A$2:$A$9</c:f>
+              <c:f>LC_alea!$A$3:$A$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0.2</c:v>
                 </c:pt>
@@ -1672,16 +1789,28 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0.55</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>LC_alea!$B$2:$B$9</c:f>
+              <c:f>LC_alea!$B$3:$B$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>447.0</c:v>
                 </c:pt>
@@ -1704,6 +1833,18 @@
                   <c:v>447.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>447.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>447.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>447.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>447.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>447.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1730,10 +1871,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>LC_alea!$A$2:$A$9</c:f>
+              <c:f>LC_alea!$A$3:$A$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0.2</c:v>
                 </c:pt>
@@ -1757,39 +1898,63 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0.55</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>LC_alea!$C$2:$C$9</c:f>
+              <c:f>LC_alea!$C$3:$C$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>483.444</c:v>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>485.174</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>504.074</c:v>
+                  <c:v>502.938</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>529.917</c:v>
+                  <c:v>537.925</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>496.815</c:v>
+                  <c:v>550.366</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>495.0</c:v>
+                  <c:v>528.6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>491.842</c:v>
+                  <c:v>570.188</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>550.4</c:v>
+                  <c:v>543.34</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>486.579</c:v>
+                  <c:v>506.778</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>540.568</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>719.3869999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>562.545</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>590.636</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1815,10 +1980,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>LC_alea!$A$2:$A$9</c:f>
+              <c:f>LC_alea!$A$3:$A$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0.2</c:v>
                 </c:pt>
@@ -1842,39 +2007,63 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0.55</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>LC_alea!$D$2:$D$9</c:f>
+              <c:f>LC_alea!$D$3:$D$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>474.0</c:v>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>471.957</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>482.296</c:v>
+                  <c:v>478.015</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>492.5</c:v>
+                  <c:v>491.473</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>488.333</c:v>
+                  <c:v>488.927</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>493.875</c:v>
+                  <c:v>492.382</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>492.0</c:v>
+                  <c:v>519.9059999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>543.8</c:v>
+                  <c:v>539.528</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>523.947</c:v>
+                  <c:v>520.704</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>549.432</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>555.645</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>552.364</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>510.273</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1900,10 +2089,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>LC_alea!$A$2:$A$9</c:f>
+              <c:f>LC_alea!$A$3:$A$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0.2</c:v>
                 </c:pt>
@@ -1927,39 +2116,63 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0.55</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>LC_alea!$E$2:$E$9</c:f>
+              <c:f>LC_alea!$E$3:$E$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>474.778</c:v>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>473.348</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>543.8150000000001</c:v>
+                  <c:v>529.985</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>507.222</c:v>
+                  <c:v>508.677</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>518.63</c:v>
+                  <c:v>527.195</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>541.062</c:v>
+                  <c:v>600.855</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>547.737</c:v>
+                  <c:v>658.4690000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>573.4</c:v>
+                  <c:v>878.585</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>655.737</c:v>
+                  <c:v>627.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>530.405</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>592.355</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>798.545</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1093.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1985,10 +2198,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>LC_alea!$A$2:$A$9</c:f>
+              <c:f>LC_alea!$A$3:$A$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0.2</c:v>
                 </c:pt>
@@ -2012,39 +2225,63 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0.55</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>LC_alea!$F$2:$F$9</c:f>
+              <c:f>LC_alea!$F$3:$F$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>477.889</c:v>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>481.435</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>494.296</c:v>
+                  <c:v>491.154</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>490.667</c:v>
+                  <c:v>493.28</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>503.704</c:v>
+                  <c:v>509.146</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>508.938</c:v>
+                  <c:v>504.6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>513.789</c:v>
+                  <c:v>517.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>502.533</c:v>
+                  <c:v>507.755</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>557.947</c:v>
+                  <c:v>541.074</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>532.784</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>541.8390000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>601.364</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>586.818</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2070,10 +2307,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>LC_alea!$A$2:$A$9</c:f>
+              <c:f>LC_alea!$A$3:$A$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0.2</c:v>
                 </c:pt>
@@ -2097,39 +2334,63 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0.55</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>LC_alea!$G$2:$G$9</c:f>
+              <c:f>LC_alea!$G$3:$G$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>479.778</c:v>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>481.522</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>494.481</c:v>
+                  <c:v>491.338</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>490.972</c:v>
+                  <c:v>493.323</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>504.444</c:v>
+                  <c:v>507.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>510.5</c:v>
+                  <c:v>506.055</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>518.895</c:v>
+                  <c:v>521.75</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>504.933</c:v>
+                  <c:v>511.679</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>557.737</c:v>
+                  <c:v>540.926</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>533.27</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>540.613</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>589.364</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>547.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2146,21 +2407,40 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2049735304"/>
-        <c:axId val="2049738440"/>
+        <c:axId val="2097989400"/>
+        <c:axId val="2097992536"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2049735304"/>
+        <c:axId val="2097989400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR"/>
+                  <a:t>Densité du graphe</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2049738440"/>
+        <c:crossAx val="2097992536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2168,20 +2448,46 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2049738440"/>
+        <c:axId val="2097992536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="650.0"/>
           <c:min val="430.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR"/>
+                  <a:t>LC</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="fr-FR" baseline="0"/>
+                  <a:t> : t</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="fr-FR"/>
+                  <a:t>ime to connectivity loss</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2049735304"/>
+        <c:crossAx val="2097989400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2887,21 +3193,40 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2045938296"/>
-        <c:axId val="2020294168"/>
+        <c:axId val="2098045832"/>
+        <c:axId val="2098048968"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2045938296"/>
+        <c:axId val="2098045832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR"/>
+                  <a:t>Densité du graphe</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2020294168"/>
+        <c:crossAx val="2098048968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2909,7 +3234,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2020294168"/>
+        <c:axId val="2098048968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="550.0"/>
@@ -2917,11 +3242,35 @@
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR"/>
+                  <a:t>Time</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="fr-FR" baseline="0"/>
+                  <a:t> To First Fall</a:t>
+                </a:r>
+                <a:endParaRPr lang="fr-FR"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2045938296"/>
+        <c:crossAx val="2098045832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3627,21 +3976,40 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2058433736"/>
-        <c:axId val="2056043416"/>
+        <c:axId val="2092188920"/>
+        <c:axId val="2092185768"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2058433736"/>
+        <c:axId val="2092188920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR"/>
+                  <a:t>Densité du graphe</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2056043416"/>
+        <c:crossAx val="2092185768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3649,18 +4017,38 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2056043416"/>
+        <c:axId val="2092185768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="500.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR"/>
+                  <a:t>PCN : time to 25% fall</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2058433736"/>
+        <c:crossAx val="2092188920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4474,21 +4862,40 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2054311448"/>
-        <c:axId val="2060163736"/>
+        <c:axId val="2098057480"/>
+        <c:axId val="2098060616"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2054311448"/>
+        <c:axId val="2098057480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR"/>
+                  <a:t>Densité du graphe</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2060163736"/>
+        <c:crossAx val="2098060616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4496,19 +4903,39 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2060163736"/>
+        <c:axId val="2098060616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1050.0"/>
           <c:min val="550.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR"/>
+                  <a:t>LC : time to connectivity loss</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2054311448"/>
+        <c:crossAx val="2098057480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5065,7 +5492,7 @@
   <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5092,392 +5519,415 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="B2">
         <v>447</v>
       </c>
       <c r="C2">
-        <v>466.9</v>
+        <v>459</v>
       </c>
       <c r="D2">
-        <v>466.4</v>
+        <v>457</v>
       </c>
       <c r="E2">
-        <v>476.5</v>
+        <v>459</v>
       </c>
       <c r="F2">
-        <v>473.8</v>
+        <v>469</v>
       </c>
       <c r="G2">
-        <v>475.4</v>
+        <v>473</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3">
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
       <c r="B3">
         <v>447</v>
       </c>
       <c r="C3">
-        <v>468.37900000000002</v>
+        <v>465</v>
       </c>
       <c r="D3">
-        <v>467.24099999999999</v>
+        <v>464.48099999999999</v>
       </c>
       <c r="E3">
-        <v>483.17200000000003</v>
+        <v>476.48099999999999</v>
       </c>
       <c r="F3">
-        <v>476.44799999999998</v>
+        <v>476.25900000000001</v>
       </c>
       <c r="G3">
-        <v>478.06900000000002</v>
+        <v>476.92599999999999</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4">
-        <v>0.3</v>
+        <v>0.25</v>
       </c>
       <c r="B4">
         <v>447</v>
       </c>
       <c r="C4">
-        <v>468.03800000000001</v>
+        <v>466.77100000000002</v>
       </c>
       <c r="D4">
-        <v>467.50599999999997</v>
+        <v>465.51400000000001</v>
       </c>
       <c r="E4">
-        <v>485.81</v>
+        <v>480.029</v>
       </c>
       <c r="F4">
-        <v>475.43</v>
+        <v>475.57100000000003</v>
       </c>
       <c r="G4">
-        <v>476.899</v>
+        <v>477.17099999999999</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5">
-        <v>0.35</v>
+        <v>0.3</v>
       </c>
       <c r="B5">
         <v>447</v>
       </c>
       <c r="C5">
-        <v>469.90899999999999</v>
+        <v>468.35300000000001</v>
       </c>
       <c r="D5">
-        <v>468.45499999999998</v>
+        <v>468.11799999999999</v>
       </c>
       <c r="E5">
-        <v>490.303</v>
+        <v>485.70600000000002</v>
       </c>
       <c r="F5">
-        <v>474.36399999999998</v>
+        <v>475.19600000000003</v>
       </c>
       <c r="G5">
-        <v>476.15199999999999</v>
+        <v>476.70600000000002</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6">
-        <v>0.4</v>
+        <v>0.35</v>
       </c>
       <c r="B6">
         <v>447</v>
       </c>
       <c r="C6">
-        <v>474.66699999999997</v>
+        <v>469.55700000000002</v>
       </c>
       <c r="D6">
-        <v>474.44400000000002</v>
+        <v>467.96899999999999</v>
       </c>
       <c r="E6">
-        <v>497.77800000000002</v>
+        <v>489.45400000000001</v>
       </c>
       <c r="F6">
-        <v>484.16699999999997</v>
+        <v>474.85599999999999</v>
       </c>
       <c r="G6">
-        <v>486.77800000000002</v>
+        <v>476.23700000000002</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7">
-        <v>0.45</v>
+        <v>0.4</v>
       </c>
       <c r="B7">
         <v>447</v>
       </c>
       <c r="C7">
-        <v>483.18200000000002</v>
+        <v>474.65600000000001</v>
       </c>
       <c r="D7">
-        <v>483.98200000000003</v>
+        <v>474.65600000000001</v>
       </c>
       <c r="E7">
-        <v>497.61799999999999</v>
+        <v>497.65600000000001</v>
       </c>
       <c r="F7">
-        <v>481.36399999999998</v>
+        <v>481.59399999999999</v>
       </c>
       <c r="G7">
-        <v>483.47300000000001</v>
+        <v>483.34399999999999</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8">
-        <v>0.5</v>
+        <v>0.45</v>
       </c>
       <c r="B8">
         <v>447</v>
       </c>
       <c r="C8">
-        <v>481.88499999999999</v>
+        <v>484.76799999999997</v>
       </c>
       <c r="D8">
-        <v>482.46199999999999</v>
+        <v>485.34800000000001</v>
       </c>
       <c r="E8">
-        <v>508.76900000000001</v>
+        <v>500.44900000000001</v>
       </c>
       <c r="F8">
-        <v>481.69200000000001</v>
+        <v>482.50700000000001</v>
       </c>
       <c r="G8">
-        <v>484.61500000000001</v>
+        <v>484.76799999999997</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9">
-        <v>0.55000000000000004</v>
+        <v>0.5</v>
       </c>
       <c r="B9">
         <v>447</v>
       </c>
       <c r="C9">
-        <v>486.37900000000002</v>
+        <v>481.09199999999998</v>
       </c>
       <c r="D9">
-        <v>490.44799999999998</v>
+        <v>483.09199999999998</v>
       </c>
       <c r="E9">
-        <v>510.24099999999999</v>
+        <v>505.64600000000002</v>
       </c>
       <c r="F9">
-        <v>483.55200000000002</v>
+        <v>481.36900000000003</v>
       </c>
       <c r="G9">
-        <v>485.06900000000002</v>
+        <v>484.04599999999999</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10">
-        <v>0.6</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="B10">
         <v>447</v>
       </c>
       <c r="C10">
-        <v>493.512</v>
+        <v>486.93900000000002</v>
       </c>
       <c r="D10">
-        <v>499.32600000000002</v>
+        <v>490.63600000000002</v>
       </c>
       <c r="E10">
-        <v>518.53499999999997</v>
+        <v>510.57600000000002</v>
       </c>
       <c r="F10">
-        <v>492.62799999999999</v>
+        <v>484.75799999999998</v>
       </c>
       <c r="G10">
-        <v>495.14</v>
+        <v>486.33300000000003</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11">
-        <v>0.65</v>
+        <v>0.6</v>
       </c>
       <c r="B11">
         <v>447</v>
       </c>
       <c r="C11">
-        <v>510.48599999999999</v>
+        <v>492.733</v>
       </c>
       <c r="D11">
-        <v>512.94299999999998</v>
+        <v>498.2</v>
       </c>
       <c r="E11">
-        <v>541.57100000000003</v>
+        <v>518.95600000000002</v>
       </c>
       <c r="F11">
-        <v>497.85700000000003</v>
+        <v>491.178</v>
       </c>
       <c r="G11">
-        <v>499.51400000000001</v>
+        <v>493.57799999999997</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12">
-        <v>0.7</v>
+        <v>0.65</v>
       </c>
       <c r="B12">
         <v>447</v>
       </c>
       <c r="C12">
-        <v>502.161</v>
+        <v>509.71800000000002</v>
       </c>
       <c r="D12">
-        <v>516.80600000000004</v>
+        <v>511.66699999999997</v>
       </c>
       <c r="E12">
-        <v>542.09699999999998</v>
+        <v>541</v>
       </c>
       <c r="F12">
-        <v>491</v>
+        <v>498.12799999999999</v>
       </c>
       <c r="G12">
-        <v>493.774</v>
+        <v>499.35899999999998</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13">
-        <v>0.75</v>
+        <v>0.7</v>
       </c>
       <c r="B13">
         <v>447</v>
       </c>
       <c r="C13">
-        <v>501.85700000000003</v>
+        <v>501.5</v>
       </c>
       <c r="D13">
-        <v>501</v>
+        <v>515.625</v>
       </c>
       <c r="E13">
-        <v>550.14300000000003</v>
+        <v>540.375</v>
       </c>
       <c r="F13">
-        <v>499.42899999999997</v>
+        <v>491.81200000000001</v>
       </c>
       <c r="G13">
-        <v>507.14299999999997</v>
+        <v>494.5</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14">
-        <v>0.8</v>
+        <v>0.75</v>
       </c>
       <c r="B14">
         <v>447</v>
       </c>
       <c r="C14">
-        <v>518.11099999999999</v>
+        <v>501.85700000000003</v>
       </c>
       <c r="D14">
-        <v>537.66700000000003</v>
+        <v>501</v>
       </c>
       <c r="E14">
-        <v>551.22199999999998</v>
+        <v>550.14300000000003</v>
       </c>
       <c r="F14">
-        <v>505.22199999999998</v>
+        <v>499.42899999999997</v>
       </c>
       <c r="G14">
-        <v>507.88900000000001</v>
+        <v>507.14299999999997</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15">
-        <v>0.85</v>
+        <v>0.8</v>
       </c>
       <c r="B15">
         <v>447</v>
       </c>
       <c r="C15">
-        <v>506.77800000000002</v>
+        <v>518.11099999999999</v>
       </c>
       <c r="D15">
-        <v>512.33299999999997</v>
+        <v>537.66700000000003</v>
       </c>
       <c r="E15">
-        <v>532.55600000000004</v>
+        <v>551.22199999999998</v>
       </c>
       <c r="F15">
-        <v>491.22199999999998</v>
+        <v>505.22199999999998</v>
       </c>
       <c r="G15">
-        <v>493.88900000000001</v>
+        <v>507.88900000000001</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16">
-        <v>0.9</v>
+        <v>0.85</v>
       </c>
       <c r="B16">
         <v>447</v>
       </c>
       <c r="C16">
-        <v>523</v>
+        <v>506.77800000000002</v>
       </c>
       <c r="D16">
-        <v>521</v>
+        <v>512.33299999999997</v>
       </c>
       <c r="E16">
-        <v>631</v>
+        <v>532.55600000000004</v>
       </c>
       <c r="F16">
-        <v>471</v>
+        <v>491.22199999999998</v>
       </c>
       <c r="G16">
-        <v>485</v>
+        <v>493.88900000000001</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17">
-        <v>0.95</v>
+        <v>0.9</v>
       </c>
       <c r="B17">
         <v>447</v>
       </c>
       <c r="C17">
-        <v>520</v>
+        <v>523</v>
       </c>
       <c r="D17">
-        <v>518</v>
+        <v>521</v>
       </c>
       <c r="E17">
-        <v>572</v>
+        <v>631</v>
       </c>
       <c r="F17">
-        <v>494</v>
+        <v>471</v>
       </c>
       <c r="G17">
-        <v>494</v>
+        <v>485</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="B18">
         <v>447</v>
       </c>
       <c r="C18">
+        <v>520</v>
+      </c>
+      <c r="D18">
+        <v>518</v>
+      </c>
+      <c r="E18">
+        <v>572</v>
+      </c>
+      <c r="F18">
+        <v>494</v>
+      </c>
+      <c r="G18">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19">
+        <v>447</v>
+      </c>
+      <c r="C19">
         <v>511</v>
       </c>
-      <c r="D18">
+      <c r="D19">
         <v>509</v>
       </c>
-      <c r="E18">
+      <c r="E19">
         <v>513</v>
       </c>
-      <c r="F18">
+      <c r="F19">
         <v>515</v>
       </c>
-      <c r="G18">
+      <c r="G19">
         <v>515</v>
       </c>
     </row>
@@ -5540,10 +5990,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5599,19 +6049,19 @@
         <v>447</v>
       </c>
       <c r="C3">
-        <v>1108</v>
+        <v>1063.57</v>
       </c>
       <c r="D3">
-        <v>1109</v>
+        <v>1072.71</v>
       </c>
       <c r="E3">
-        <v>4905.33</v>
+        <v>4822.1400000000003</v>
       </c>
       <c r="F3">
-        <v>1222.33</v>
+        <v>1317.86</v>
       </c>
       <c r="G3">
-        <v>1433</v>
+        <v>1561.57</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -5622,19 +6072,19 @@
         <v>447</v>
       </c>
       <c r="C4">
-        <v>1085.33</v>
+        <v>1080.8599999999999</v>
       </c>
       <c r="D4">
-        <v>1244</v>
+        <v>1298.71</v>
       </c>
       <c r="E4">
-        <v>5448.83</v>
+        <v>5447.71</v>
       </c>
       <c r="F4">
-        <v>1470.33</v>
+        <v>1474.43</v>
       </c>
       <c r="G4">
-        <v>1619.17</v>
+        <v>1622</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -5645,19 +6095,19 @@
         <v>447</v>
       </c>
       <c r="C5">
-        <v>1063.18</v>
+        <v>1054.29</v>
       </c>
       <c r="D5">
-        <v>1325.45</v>
+        <v>1342.14</v>
       </c>
       <c r="E5">
-        <v>5559.45</v>
+        <v>5604.5</v>
       </c>
       <c r="F5">
-        <v>1294</v>
+        <v>1311</v>
       </c>
       <c r="G5">
-        <v>1417.27</v>
+        <v>1421.86</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -5668,19 +6118,19 @@
         <v>447</v>
       </c>
       <c r="C6">
-        <v>1033.8599999999999</v>
+        <v>1013.26</v>
       </c>
       <c r="D6">
-        <v>1534.81</v>
+        <v>1456.48</v>
       </c>
       <c r="E6">
-        <v>6630.33</v>
+        <v>6801.26</v>
       </c>
       <c r="F6">
-        <v>1411.57</v>
+        <v>1401.65</v>
       </c>
       <c r="G6">
-        <v>1661.19</v>
+        <v>1579.97</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -5691,19 +6141,19 @@
         <v>447</v>
       </c>
       <c r="C7">
-        <v>1152.54</v>
+        <v>1132.76</v>
       </c>
       <c r="D7">
-        <v>1301</v>
+        <v>1378.53</v>
       </c>
       <c r="E7">
-        <v>6235</v>
+        <v>6443.94</v>
       </c>
       <c r="F7">
-        <v>1285.46</v>
+        <v>1340.29</v>
       </c>
       <c r="G7">
-        <v>1382.85</v>
+        <v>1489.12</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -5714,19 +6164,19 @@
         <v>447</v>
       </c>
       <c r="C8">
-        <v>1103.5999999999999</v>
+        <v>1077</v>
       </c>
       <c r="D8">
-        <v>1288.4000000000001</v>
+        <v>1330.08</v>
       </c>
       <c r="E8">
-        <v>6672.6</v>
+        <v>6788.38</v>
       </c>
       <c r="F8">
-        <v>1157.8</v>
+        <v>1181.1500000000001</v>
       </c>
       <c r="G8">
-        <v>1508.6</v>
+        <v>1448.23</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -5737,19 +6187,19 @@
         <v>447</v>
       </c>
       <c r="C9">
-        <v>1203</v>
+        <v>1061.5</v>
       </c>
       <c r="D9">
-        <v>1839</v>
+        <v>1558.5</v>
       </c>
       <c r="E9">
-        <v>9254</v>
+        <v>8281</v>
       </c>
       <c r="F9">
-        <v>1304</v>
+        <v>1219</v>
       </c>
       <c r="G9">
-        <v>1525</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -5760,19 +6210,65 @@
         <v>447</v>
       </c>
       <c r="C10">
-        <v>1001</v>
+        <v>965</v>
       </c>
       <c r="D10">
-        <v>1395</v>
+        <v>1363</v>
       </c>
       <c r="E10">
-        <v>6269</v>
+        <v>6199</v>
       </c>
       <c r="F10">
-        <v>2081</v>
+        <v>1410.33</v>
       </c>
       <c r="G10">
-        <v>2587</v>
+        <v>1601.67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11">
+        <v>0.6</v>
+      </c>
+      <c r="B11">
+        <v>447</v>
+      </c>
+      <c r="C11">
+        <v>831</v>
+      </c>
+      <c r="D11">
+        <v>1245</v>
+      </c>
+      <c r="E11">
+        <v>6427</v>
+      </c>
+      <c r="F11">
+        <v>1507</v>
+      </c>
+      <c r="G11">
+        <v>1449</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12">
+        <v>0.65</v>
+      </c>
+      <c r="B12">
+        <v>447</v>
+      </c>
+      <c r="C12">
+        <v>1079</v>
+      </c>
+      <c r="D12">
+        <v>1801</v>
+      </c>
+      <c r="E12">
+        <v>5637</v>
+      </c>
+      <c r="F12">
+        <v>1117</v>
+      </c>
+      <c r="G12">
+        <v>1213</v>
       </c>
     </row>
   </sheetData>
@@ -5789,10 +6285,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5819,392 +6315,415 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="B2">
         <v>447</v>
       </c>
       <c r="C2">
-        <v>483.44400000000002</v>
+        <v>6505</v>
       </c>
       <c r="D2">
-        <v>474</v>
+        <v>457</v>
       </c>
       <c r="E2">
-        <v>474.77800000000002</v>
+        <v>459</v>
       </c>
       <c r="F2">
-        <v>477.88900000000001</v>
+        <v>469</v>
       </c>
       <c r="G2">
-        <v>479.77800000000002</v>
+        <v>473</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3">
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
       <c r="B3">
         <v>447</v>
       </c>
       <c r="C3">
-        <v>504.07400000000001</v>
+        <v>485.17399999999998</v>
       </c>
       <c r="D3">
-        <v>482.29599999999999</v>
+        <v>471.95699999999999</v>
       </c>
       <c r="E3">
-        <v>543.81500000000005</v>
+        <v>473.34800000000001</v>
       </c>
       <c r="F3">
-        <v>494.29599999999999</v>
+        <v>481.435</v>
       </c>
       <c r="G3">
-        <v>494.48099999999999</v>
+        <v>481.52199999999999</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4">
-        <v>0.3</v>
+        <v>0.25</v>
       </c>
       <c r="B4">
         <v>447</v>
       </c>
       <c r="C4">
-        <v>529.91700000000003</v>
+        <v>502.93799999999999</v>
       </c>
       <c r="D4">
-        <v>492.5</v>
+        <v>478.01499999999999</v>
       </c>
       <c r="E4">
-        <v>507.22199999999998</v>
+        <v>529.98500000000001</v>
       </c>
       <c r="F4">
-        <v>490.66699999999997</v>
+        <v>491.154</v>
       </c>
       <c r="G4">
-        <v>490.97199999999998</v>
+        <v>491.33800000000002</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5">
-        <v>0.35</v>
+        <v>0.3</v>
       </c>
       <c r="B5">
         <v>447</v>
       </c>
       <c r="C5">
-        <v>496.815</v>
+        <v>537.92499999999995</v>
       </c>
       <c r="D5">
-        <v>488.33300000000003</v>
+        <v>491.47300000000001</v>
       </c>
       <c r="E5">
-        <v>518.63</v>
+        <v>508.67700000000002</v>
       </c>
       <c r="F5">
-        <v>503.70400000000001</v>
+        <v>493.28</v>
       </c>
       <c r="G5">
-        <v>504.44400000000002</v>
+        <v>493.32299999999998</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6">
-        <v>0.4</v>
+        <v>0.35</v>
       </c>
       <c r="B6">
         <v>447</v>
       </c>
       <c r="C6">
-        <v>495</v>
+        <v>550.36599999999999</v>
       </c>
       <c r="D6">
-        <v>493.875</v>
+        <v>488.92700000000002</v>
       </c>
       <c r="E6">
-        <v>541.06200000000001</v>
+        <v>527.19500000000005</v>
       </c>
       <c r="F6">
-        <v>508.93799999999999</v>
+        <v>509.14600000000002</v>
       </c>
       <c r="G6">
-        <v>510.5</v>
+        <v>507</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7">
-        <v>0.45</v>
+        <v>0.4</v>
       </c>
       <c r="B7">
         <v>447</v>
       </c>
       <c r="C7">
-        <v>491.84199999999998</v>
+        <v>528.6</v>
       </c>
       <c r="D7">
-        <v>492</v>
+        <v>492.38200000000001</v>
       </c>
       <c r="E7">
-        <v>547.73699999999997</v>
+        <v>600.85500000000002</v>
       </c>
       <c r="F7">
-        <v>513.78899999999999</v>
+        <v>504.6</v>
       </c>
       <c r="G7">
-        <v>518.89499999999998</v>
+        <v>506.05500000000001</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8">
-        <v>0.5</v>
+        <v>0.45</v>
       </c>
       <c r="B8">
         <v>447</v>
       </c>
       <c r="C8">
-        <v>550.4</v>
+        <v>570.18799999999999</v>
       </c>
       <c r="D8">
-        <v>543.79999999999995</v>
+        <v>519.90599999999995</v>
       </c>
       <c r="E8">
-        <v>573.4</v>
+        <v>658.46900000000005</v>
       </c>
       <c r="F8">
-        <v>502.53300000000002</v>
+        <v>517</v>
       </c>
       <c r="G8">
-        <v>504.93299999999999</v>
+        <v>521.75</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9">
-        <v>0.55000000000000004</v>
+        <v>0.5</v>
       </c>
       <c r="B9">
         <v>447</v>
       </c>
       <c r="C9">
-        <v>486.57900000000001</v>
+        <v>543.34</v>
       </c>
       <c r="D9">
-        <v>523.947</v>
+        <v>539.52800000000002</v>
       </c>
       <c r="E9">
-        <v>655.73699999999997</v>
+        <v>878.58500000000004</v>
       </c>
       <c r="F9">
-        <v>557.947</v>
+        <v>507.755</v>
       </c>
       <c r="G9">
-        <v>557.73699999999997</v>
+        <v>511.67899999999997</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10">
-        <v>0.6</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="B10">
         <v>447</v>
       </c>
       <c r="C10">
-        <v>535</v>
+        <v>506.77800000000002</v>
       </c>
       <c r="D10">
-        <v>552.93299999999999</v>
+        <v>520.70399999999995</v>
       </c>
       <c r="E10">
-        <v>532.26700000000005</v>
+        <v>627</v>
       </c>
       <c r="F10">
-        <v>532.66700000000003</v>
+        <v>541.07399999999996</v>
       </c>
       <c r="G10">
-        <v>533.46699999999998</v>
+        <v>540.92600000000004</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11">
-        <v>0.65</v>
+        <v>0.6</v>
       </c>
       <c r="B11">
         <v>447</v>
       </c>
       <c r="C11">
-        <v>735.72</v>
+        <v>540.56799999999998</v>
       </c>
       <c r="D11">
-        <v>556.04</v>
+        <v>549.43200000000002</v>
       </c>
       <c r="E11">
-        <v>597.48</v>
+        <v>530.40499999999997</v>
       </c>
       <c r="F11">
-        <v>534.76</v>
+        <v>532.78399999999999</v>
       </c>
       <c r="G11">
-        <v>530.20000000000005</v>
+        <v>533.27</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12">
-        <v>0.7</v>
+        <v>0.65</v>
       </c>
       <c r="B12">
         <v>447</v>
       </c>
       <c r="C12">
-        <v>562.54499999999996</v>
+        <v>719.38699999999994</v>
       </c>
       <c r="D12">
-        <v>552.36400000000003</v>
+        <v>555.64499999999998</v>
       </c>
       <c r="E12">
-        <v>798.54499999999996</v>
+        <v>592.35500000000002</v>
       </c>
       <c r="F12">
-        <v>601.36400000000003</v>
+        <v>541.83900000000006</v>
       </c>
       <c r="G12">
-        <v>589.36400000000003</v>
+        <v>540.61300000000006</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13">
-        <v>0.75</v>
+        <v>0.7</v>
       </c>
       <c r="B13">
         <v>447</v>
       </c>
       <c r="C13">
-        <v>590.63599999999997</v>
+        <v>562.54499999999996</v>
       </c>
       <c r="D13">
-        <v>510.27300000000002</v>
+        <v>552.36400000000003</v>
       </c>
       <c r="E13">
-        <v>1093</v>
+        <v>798.54499999999996</v>
       </c>
       <c r="F13">
-        <v>586.81799999999998</v>
+        <v>601.36400000000003</v>
       </c>
       <c r="G13">
-        <v>547</v>
+        <v>589.36400000000003</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14">
-        <v>0.8</v>
+        <v>0.75</v>
       </c>
       <c r="B14">
         <v>447</v>
       </c>
       <c r="C14">
-        <v>475.66699999999997</v>
+        <v>590.63599999999997</v>
       </c>
       <c r="D14">
-        <v>826.33299999999997</v>
+        <v>510.27300000000002</v>
       </c>
       <c r="E14">
-        <v>3943.67</v>
+        <v>1093</v>
       </c>
       <c r="F14">
-        <v>634.33299999999997</v>
+        <v>586.81799999999998</v>
       </c>
       <c r="G14">
-        <v>677</v>
+        <v>547</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15">
-        <v>0.85</v>
+        <v>0.8</v>
       </c>
       <c r="B15">
         <v>447</v>
       </c>
       <c r="C15">
-        <v>509</v>
+        <v>475.66699999999997</v>
       </c>
       <c r="D15">
-        <v>746.25</v>
+        <v>826.33299999999997</v>
       </c>
       <c r="E15">
-        <v>2100</v>
+        <v>3943.67</v>
       </c>
       <c r="F15">
-        <v>545.75</v>
+        <v>634.33299999999997</v>
       </c>
       <c r="G15">
-        <v>549</v>
+        <v>677</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16">
-        <v>0.9</v>
+        <v>0.85</v>
       </c>
       <c r="B16">
         <v>447</v>
       </c>
       <c r="C16">
-        <v>637</v>
+        <v>509</v>
       </c>
       <c r="D16">
-        <v>687</v>
+        <v>746.25</v>
       </c>
       <c r="E16">
-        <v>9719</v>
+        <v>2100</v>
       </c>
       <c r="F16">
-        <v>593</v>
+        <v>545.75</v>
       </c>
       <c r="G16">
-        <v>607</v>
+        <v>549</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17">
-        <v>0.95</v>
+        <v>0.9</v>
       </c>
       <c r="B17">
         <v>447</v>
       </c>
       <c r="C17">
-        <v>449</v>
+        <v>637</v>
       </c>
       <c r="D17">
-        <v>525</v>
+        <v>687</v>
       </c>
       <c r="E17">
-        <v>529</v>
+        <v>9719</v>
       </c>
       <c r="F17">
-        <v>535</v>
+        <v>593</v>
       </c>
       <c r="G17">
-        <v>531</v>
+        <v>607</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="B18">
         <v>447</v>
       </c>
       <c r="C18">
+        <v>659</v>
+      </c>
+      <c r="D18">
+        <v>720</v>
+      </c>
+      <c r="E18">
+        <v>736</v>
+      </c>
+      <c r="F18">
+        <v>567</v>
+      </c>
+      <c r="G18">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19">
+        <v>447</v>
+      </c>
+      <c r="C19">
         <v>453</v>
       </c>
-      <c r="D18">
+      <c r="D19">
         <v>509</v>
       </c>
-      <c r="E18">
+      <c r="E19">
         <v>513</v>
       </c>
-      <c r="F18">
+      <c r="F19">
         <v>515</v>
       </c>
-      <c r="G18">
+      <c r="G19">
         <v>515</v>
       </c>
     </row>
@@ -7089,8 +7608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>